<commit_message>
Final settlement match logic added
</commit_message>
<xml_diff>
--- a/Resources/Steel-Trans/Steel book Trans_MATCHED.xlsx
+++ b/Resources/Steel-Trans/Steel book Trans_MATCHED.xlsx
@@ -765,7 +765,7 @@
     <row r="11">
       <c r="A11" s="9" t="inlineStr">
         <is>
-          <t>M025</t>
+          <t>M030</t>
         </is>
       </c>
       <c r="B11" s="10" t="inlineStr"/>
@@ -811,7 +811,7 @@
     <row r="12">
       <c r="A12" s="9" t="inlineStr">
         <is>
-          <t>M025</t>
+          <t>M030</t>
         </is>
       </c>
       <c r="B12" s="10" t="inlineStr">
@@ -843,7 +843,7 @@
     <row r="13">
       <c r="A13" s="9" t="inlineStr">
         <is>
-          <t>M025</t>
+          <t>M030</t>
         </is>
       </c>
       <c r="B13" s="10" t="inlineStr"/>
@@ -873,7 +873,7 @@
     <row r="14">
       <c r="A14" s="17" t="inlineStr">
         <is>
-          <t>M026</t>
+          <t>M025</t>
         </is>
       </c>
       <c r="B14" s="18" t="inlineStr"/>
@@ -912,19 +912,19 @@
       <c r="K14" s="17" t="inlineStr"/>
       <c r="L14" s="17" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="17" t="inlineStr">
         <is>
-          <t>M026</t>
+          <t>M025</t>
         </is>
       </c>
       <c r="B15" s="18" t="inlineStr">
         <is>
-          <t>Manual Match
+          <t>Settlement Match (ID: 11370) - 'Final Settlement' keyword found
 Lender Amount: 99317.00
 Borrower Amount: 99317.00</t>
         </is>
@@ -944,14 +944,14 @@
       <c r="K15" s="17" t="inlineStr"/>
       <c r="L15" s="17" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="17" t="inlineStr">
         <is>
-          <t>M026</t>
+          <t>M025</t>
         </is>
       </c>
       <c r="B16" s="18" t="inlineStr"/>
@@ -974,14 +974,14 @@
       <c r="K16" s="17" t="inlineStr"/>
       <c r="L16" s="17" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="9" t="inlineStr">
         <is>
-          <t>M027</t>
+          <t>M026</t>
         </is>
       </c>
       <c r="B17" s="10" t="inlineStr"/>
@@ -1020,19 +1020,19 @@
       <c r="K17" s="9" t="inlineStr"/>
       <c r="L17" s="9" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9" t="inlineStr">
         <is>
-          <t>M027</t>
+          <t>M026</t>
         </is>
       </c>
       <c r="B18" s="10" t="inlineStr">
         <is>
-          <t>Manual Match
+          <t>Settlement Match (ID: 10199) - 'Final Settlement' keyword found
 Lender Amount: 20130.00
 Borrower Amount: 20130.00</t>
         </is>
@@ -1052,14 +1052,14 @@
       <c r="K18" s="9" t="inlineStr"/>
       <c r="L18" s="9" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="9" t="inlineStr">
         <is>
-          <t>M027</t>
+          <t>M026</t>
         </is>
       </c>
       <c r="B19" s="10" t="inlineStr"/>
@@ -1082,14 +1082,14 @@
       <c r="K19" s="9" t="inlineStr"/>
       <c r="L19" s="9" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="17" t="inlineStr">
         <is>
-          <t>M028</t>
+          <t>M027</t>
         </is>
       </c>
       <c r="B20" s="18" t="inlineStr"/>
@@ -1128,19 +1128,19 @@
       <c r="K20" s="17" t="inlineStr"/>
       <c r="L20" s="17" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="17" t="inlineStr">
         <is>
-          <t>M028</t>
+          <t>M027</t>
         </is>
       </c>
       <c r="B21" s="18" t="inlineStr">
         <is>
-          <t>Manual Match
+          <t>Settlement Match (ID: 11711) - 'Final Settlement' keyword found
 Lender Amount: 94109.00
 Borrower Amount: 94109.00</t>
         </is>
@@ -1160,14 +1160,14 @@
       <c r="K21" s="17" t="inlineStr"/>
       <c r="L21" s="17" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="17" t="inlineStr">
         <is>
-          <t>M028</t>
+          <t>M027</t>
         </is>
       </c>
       <c r="B22" s="18" t="inlineStr"/>
@@ -1190,14 +1190,14 @@
       <c r="K22" s="17" t="inlineStr"/>
       <c r="L22" s="17" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="9" t="inlineStr">
         <is>
-          <t>M029</t>
+          <t>M028</t>
         </is>
       </c>
       <c r="B23" s="10" t="inlineStr"/>
@@ -1236,19 +1236,19 @@
       <c r="K23" s="9" t="inlineStr"/>
       <c r="L23" s="9" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="9" t="inlineStr">
         <is>
-          <t>M029</t>
+          <t>M028</t>
         </is>
       </c>
       <c r="B24" s="10" t="inlineStr">
         <is>
-          <t>Manual Match
+          <t>Settlement Match (ID: 11134) - 'Final Settlement' keyword found
 Lender Amount: 13909.00
 Borrower Amount: 13909.00</t>
         </is>
@@ -1268,14 +1268,14 @@
       <c r="K24" s="9" t="inlineStr"/>
       <c r="L24" s="9" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="9" t="inlineStr">
         <is>
-          <t>M029</t>
+          <t>M028</t>
         </is>
       </c>
       <c r="B25" s="10" t="inlineStr"/>
@@ -1298,14 +1298,14 @@
       <c r="K25" s="9" t="inlineStr"/>
       <c r="L25" s="9" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="17" t="inlineStr">
         <is>
-          <t>M030</t>
+          <t>M029</t>
         </is>
       </c>
       <c r="B26" s="18" t="inlineStr"/>
@@ -1344,19 +1344,19 @@
       <c r="K26" s="17" t="inlineStr"/>
       <c r="L26" s="17" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="17" t="inlineStr">
         <is>
-          <t>M030</t>
+          <t>M029</t>
         </is>
       </c>
       <c r="B27" s="18" t="inlineStr">
         <is>
-          <t>Manual Match
+          <t>Settlement Match (ID: 12107) - 'Final Settlement' keyword found
 Lender Amount: 93314.00
 Borrower Amount: 93314.00</t>
         </is>
@@ -1376,14 +1376,14 @@
       <c r="K27" s="17" t="inlineStr"/>
       <c r="L27" s="17" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="17" t="inlineStr">
         <is>
-          <t>M030</t>
+          <t>M029</t>
         </is>
       </c>
       <c r="B28" s="18" t="inlineStr"/>
@@ -1406,7 +1406,7 @@
       <c r="K28" s="17" t="inlineStr"/>
       <c r="L28" s="17" t="inlineStr">
         <is>
-          <t>Manual</t>
+          <t>Settlement</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Manual table design fixed
</commit_message>
<xml_diff>
--- a/Resources/Steel-Trans/Steel book Trans_MATCHED.xlsx
+++ b/Resources/Steel-Trans/Steel book Trans_MATCHED.xlsx
@@ -76,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -148,6 +148,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -3955,2742 +3964,2566 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="17" t="inlineStr">
-        <is>
-          <t>M053</t>
-        </is>
-      </c>
-      <c r="B100" s="18" t="inlineStr"/>
-      <c r="C100" s="19" t="inlineStr">
+      <c r="A100" s="1" t="inlineStr"/>
+      <c r="B100" s="2" t="inlineStr"/>
+      <c r="C100" s="6" t="inlineStr">
         <is>
           <t>03/Jun/2025</t>
         </is>
       </c>
-      <c r="D100" s="17" t="inlineStr">
+      <c r="D100" s="1" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E100" s="20" t="inlineStr">
+      <c r="E100" s="7" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F100" s="17" t="inlineStr"/>
-      <c r="G100" s="17" t="inlineStr"/>
-      <c r="H100" s="21" t="inlineStr">
+      <c r="F100" s="1" t="inlineStr"/>
+      <c r="G100" s="1" t="inlineStr"/>
+      <c r="H100" s="25" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I100" s="17" t="inlineStr">
+      <c r="I100" s="1" t="inlineStr">
         <is>
           <t>70712</t>
         </is>
       </c>
-      <c r="J100" s="22" t="inlineStr">
+      <c r="J100" s="8" t="inlineStr">
         <is>
           <t>200000</t>
         </is>
       </c>
-      <c r="K100" s="17" t="inlineStr"/>
-      <c r="L100" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="K100" s="1" t="inlineStr"/>
+      <c r="L100" s="1" t="inlineStr"/>
     </row>
     <row r="101">
-      <c r="A101" s="17" t="inlineStr">
-        <is>
-          <t>M053</t>
-        </is>
-      </c>
-      <c r="B101" s="18" t="inlineStr">
-        <is>
-          <t>Manual Match
-Lender Amount: 200000.00
-Borrower Amount: 200000.00</t>
-        </is>
-      </c>
-      <c r="C101" s="17" t="inlineStr"/>
-      <c r="D101" s="17" t="inlineStr"/>
-      <c r="E101" s="23" t="inlineStr">
+      <c r="A101" s="1" t="inlineStr"/>
+      <c r="B101" s="2" t="inlineStr">
+        <is>
+          <t>Unmatched Record
+Reasons:
+1. Borrower's narration does not contain lender's short code
+2. Settlement mismatch: File 1 IDs [], File 2 IDs ['92117']</t>
+        </is>
+      </c>
+      <c r="C101" s="1" t="inlineStr"/>
+      <c r="D101" s="1" t="inlineStr"/>
+      <c r="E101" s="26" t="inlineStr">
         <is>
           <t>Amount paid as interunit vendor payment.(M/S United Traders)</t>
         </is>
       </c>
-      <c r="F101" s="17" t="inlineStr"/>
-      <c r="G101" s="17" t="inlineStr"/>
-      <c r="H101" s="17" t="inlineStr"/>
-      <c r="I101" s="17" t="inlineStr"/>
-      <c r="J101" s="17" t="inlineStr"/>
-      <c r="K101" s="17" t="inlineStr"/>
-      <c r="L101" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F101" s="1" t="inlineStr"/>
+      <c r="G101" s="1" t="inlineStr"/>
+      <c r="H101" s="1" t="inlineStr"/>
+      <c r="I101" s="1" t="inlineStr"/>
+      <c r="J101" s="1" t="inlineStr"/>
+      <c r="K101" s="1" t="inlineStr"/>
+      <c r="L101" s="1" t="inlineStr"/>
     </row>
     <row r="102">
-      <c r="A102" s="17" t="inlineStr">
-        <is>
-          <t>M053</t>
-        </is>
-      </c>
-      <c r="B102" s="18" t="inlineStr"/>
-      <c r="C102" s="17" t="inlineStr"/>
-      <c r="D102" s="17" t="inlineStr">
+      <c r="A102" s="1" t="inlineStr"/>
+      <c r="B102" s="2" t="inlineStr"/>
+      <c r="C102" s="1" t="inlineStr"/>
+      <c r="D102" s="1" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E102" s="24" t="inlineStr">
+      <c r="E102" s="27" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F102" s="17" t="inlineStr"/>
-      <c r="G102" s="17" t="inlineStr"/>
-      <c r="H102" s="17" t="inlineStr"/>
-      <c r="I102" s="17" t="inlineStr"/>
-      <c r="J102" s="17" t="inlineStr"/>
-      <c r="K102" s="17" t="inlineStr"/>
-      <c r="L102" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F102" s="1" t="inlineStr"/>
+      <c r="G102" s="1" t="inlineStr"/>
+      <c r="H102" s="1" t="inlineStr"/>
+      <c r="I102" s="1" t="inlineStr"/>
+      <c r="J102" s="1" t="inlineStr"/>
+      <c r="K102" s="1" t="inlineStr"/>
+      <c r="L102" s="1" t="inlineStr"/>
     </row>
     <row r="103">
-      <c r="A103" s="9" t="inlineStr">
+      <c r="A103" s="17" t="inlineStr">
         <is>
           <t>M018</t>
         </is>
       </c>
-      <c r="B103" s="10" t="inlineStr"/>
-      <c r="C103" s="11" t="inlineStr">
+      <c r="B103" s="18" t="inlineStr"/>
+      <c r="C103" s="19" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D103" s="9" t="inlineStr">
+      <c r="D103" s="17" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E103" s="12" t="inlineStr">
+      <c r="E103" s="20" t="inlineStr">
         <is>
           <t>Dhaka Bank-STD-2051501833-CIL</t>
         </is>
       </c>
-      <c r="F103" s="9" t="inlineStr"/>
-      <c r="G103" s="9" t="inlineStr"/>
-      <c r="H103" s="13" t="inlineStr">
+      <c r="F103" s="17" t="inlineStr"/>
+      <c r="G103" s="17" t="inlineStr"/>
+      <c r="H103" s="21" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I103" s="9" t="inlineStr">
+      <c r="I103" s="17" t="inlineStr">
         <is>
           <t>939</t>
         </is>
       </c>
-      <c r="J103" s="9" t="inlineStr"/>
-      <c r="K103" s="14" t="inlineStr">
+      <c r="J103" s="17" t="inlineStr"/>
+      <c r="K103" s="22" t="inlineStr">
         <is>
           <t>12000000</t>
         </is>
       </c>
-      <c r="L103" s="9" t="inlineStr">
+      <c r="L103" s="17" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="9" t="inlineStr">
+      <c r="A104" s="17" t="inlineStr">
         <is>
           <t>M018</t>
         </is>
       </c>
-      <c r="B104" s="10" t="inlineStr">
+      <c r="B104" s="18" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0313
 Lender Amount: 12000000.00
 Borrower Amount: 12000000.00</t>
         </is>
       </c>
-      <c r="C104" s="9" t="inlineStr"/>
-      <c r="D104" s="9" t="inlineStr"/>
-      <c r="E104" s="15" t="inlineStr">
+      <c r="C104" s="17" t="inlineStr"/>
+      <c r="D104" s="17" t="inlineStr"/>
+      <c r="E104" s="23" t="inlineStr">
         <is>
           <t>Interunit fund Transfer as Inter Unit Loan A/C-Transformer Unit,MDB#0313</t>
         </is>
       </c>
-      <c r="F104" s="9" t="inlineStr"/>
-      <c r="G104" s="9" t="inlineStr"/>
-      <c r="H104" s="9" t="inlineStr"/>
-      <c r="I104" s="9" t="inlineStr"/>
-      <c r="J104" s="9" t="inlineStr"/>
-      <c r="K104" s="9" t="inlineStr"/>
-      <c r="L104" s="9" t="inlineStr">
+      <c r="F104" s="17" t="inlineStr"/>
+      <c r="G104" s="17" t="inlineStr"/>
+      <c r="H104" s="17" t="inlineStr"/>
+      <c r="I104" s="17" t="inlineStr"/>
+      <c r="J104" s="17" t="inlineStr"/>
+      <c r="K104" s="17" t="inlineStr"/>
+      <c r="L104" s="17" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="9" t="inlineStr">
+      <c r="A105" s="17" t="inlineStr">
         <is>
           <t>M018</t>
         </is>
       </c>
-      <c r="B105" s="10" t="inlineStr"/>
-      <c r="C105" s="9" t="inlineStr"/>
-      <c r="D105" s="9" t="inlineStr">
+      <c r="B105" s="18" t="inlineStr"/>
+      <c r="C105" s="17" t="inlineStr"/>
+      <c r="D105" s="17" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E105" s="16" t="inlineStr">
+      <c r="E105" s="24" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F105" s="9" t="inlineStr"/>
-      <c r="G105" s="9" t="inlineStr"/>
-      <c r="H105" s="9" t="inlineStr"/>
-      <c r="I105" s="9" t="inlineStr"/>
-      <c r="J105" s="9" t="inlineStr"/>
-      <c r="K105" s="9" t="inlineStr"/>
-      <c r="L105" s="9" t="inlineStr">
+      <c r="F105" s="17" t="inlineStr"/>
+      <c r="G105" s="17" t="inlineStr"/>
+      <c r="H105" s="17" t="inlineStr"/>
+      <c r="I105" s="17" t="inlineStr"/>
+      <c r="J105" s="17" t="inlineStr"/>
+      <c r="K105" s="17" t="inlineStr"/>
+      <c r="L105" s="17" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="17" t="inlineStr">
+      <c r="A106" s="9" t="inlineStr">
         <is>
           <t>M019</t>
         </is>
       </c>
-      <c r="B106" s="18" t="inlineStr"/>
-      <c r="C106" s="19" t="inlineStr">
+      <c r="B106" s="10" t="inlineStr"/>
+      <c r="C106" s="11" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D106" s="17" t="inlineStr">
+      <c r="D106" s="9" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E106" s="20" t="inlineStr">
+      <c r="E106" s="12" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F106" s="17" t="inlineStr"/>
-      <c r="G106" s="17" t="inlineStr"/>
-      <c r="H106" s="21" t="inlineStr">
+      <c r="F106" s="9" t="inlineStr"/>
+      <c r="G106" s="9" t="inlineStr"/>
+      <c r="H106" s="13" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I106" s="17" t="inlineStr">
+      <c r="I106" s="9" t="inlineStr">
         <is>
           <t>940</t>
         </is>
       </c>
-      <c r="J106" s="17" t="inlineStr"/>
-      <c r="K106" s="22" t="inlineStr">
+      <c r="J106" s="9" t="inlineStr"/>
+      <c r="K106" s="14" t="inlineStr">
         <is>
           <t>22000000</t>
         </is>
       </c>
-      <c r="L106" s="17" t="inlineStr">
+      <c r="L106" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="17" t="inlineStr">
+      <c r="A107" s="9" t="inlineStr">
         <is>
           <t>M019</t>
         </is>
       </c>
-      <c r="B107" s="18" t="inlineStr">
+      <c r="B107" s="10" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0313
 Lender Amount: 22000000.00
 Borrower Amount: 22000000.00</t>
         </is>
       </c>
-      <c r="C107" s="17" t="inlineStr"/>
-      <c r="D107" s="17" t="inlineStr"/>
-      <c r="E107" s="23" t="inlineStr">
+      <c r="C107" s="9" t="inlineStr"/>
+      <c r="D107" s="9" t="inlineStr"/>
+      <c r="E107" s="15" t="inlineStr">
         <is>
           <t>Interunit fund Transfer as Inter Unit Loan A/C-Transformer Unit,MDB#0313</t>
         </is>
       </c>
-      <c r="F107" s="17" t="inlineStr"/>
-      <c r="G107" s="17" t="inlineStr"/>
-      <c r="H107" s="17" t="inlineStr"/>
-      <c r="I107" s="17" t="inlineStr"/>
-      <c r="J107" s="17" t="inlineStr"/>
-      <c r="K107" s="17" t="inlineStr"/>
-      <c r="L107" s="17" t="inlineStr">
+      <c r="F107" s="9" t="inlineStr"/>
+      <c r="G107" s="9" t="inlineStr"/>
+      <c r="H107" s="9" t="inlineStr"/>
+      <c r="I107" s="9" t="inlineStr"/>
+      <c r="J107" s="9" t="inlineStr"/>
+      <c r="K107" s="9" t="inlineStr"/>
+      <c r="L107" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="17" t="inlineStr">
+      <c r="A108" s="9" t="inlineStr">
         <is>
           <t>M019</t>
         </is>
       </c>
-      <c r="B108" s="18" t="inlineStr"/>
-      <c r="C108" s="17" t="inlineStr"/>
-      <c r="D108" s="17" t="inlineStr">
+      <c r="B108" s="10" t="inlineStr"/>
+      <c r="C108" s="9" t="inlineStr"/>
+      <c r="D108" s="9" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E108" s="24" t="inlineStr">
+      <c r="E108" s="16" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F108" s="17" t="inlineStr"/>
-      <c r="G108" s="17" t="inlineStr"/>
-      <c r="H108" s="17" t="inlineStr"/>
-      <c r="I108" s="17" t="inlineStr"/>
-      <c r="J108" s="17" t="inlineStr"/>
-      <c r="K108" s="17" t="inlineStr"/>
-      <c r="L108" s="17" t="inlineStr">
+      <c r="F108" s="9" t="inlineStr"/>
+      <c r="G108" s="9" t="inlineStr"/>
+      <c r="H108" s="9" t="inlineStr"/>
+      <c r="I108" s="9" t="inlineStr"/>
+      <c r="J108" s="9" t="inlineStr"/>
+      <c r="K108" s="9" t="inlineStr"/>
+      <c r="L108" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="9" t="inlineStr">
-        <is>
-          <t>M056</t>
-        </is>
-      </c>
-      <c r="B109" s="10" t="inlineStr"/>
-      <c r="C109" s="11" t="inlineStr">
+      <c r="A109" s="1" t="inlineStr"/>
+      <c r="B109" s="2" t="inlineStr"/>
+      <c r="C109" s="6" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D109" s="9" t="inlineStr">
+      <c r="D109" s="1" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E109" s="12" t="inlineStr">
+      <c r="E109" s="7" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F109" s="9" t="inlineStr"/>
-      <c r="G109" s="9" t="inlineStr"/>
-      <c r="H109" s="13" t="inlineStr">
+      <c r="F109" s="1" t="inlineStr"/>
+      <c r="G109" s="1" t="inlineStr"/>
+      <c r="H109" s="25" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I109" s="9" t="inlineStr">
+      <c r="I109" s="1" t="inlineStr">
         <is>
           <t>70714</t>
         </is>
       </c>
-      <c r="J109" s="14" t="inlineStr">
+      <c r="J109" s="8" t="inlineStr">
         <is>
           <t>58108</t>
         </is>
       </c>
-      <c r="K109" s="9" t="inlineStr"/>
-      <c r="L109" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="K109" s="1" t="inlineStr"/>
+      <c r="L109" s="1" t="inlineStr"/>
     </row>
     <row r="110">
-      <c r="A110" s="9" t="inlineStr">
-        <is>
-          <t>M056</t>
-        </is>
-      </c>
-      <c r="B110" s="10" t="inlineStr">
-        <is>
-          <t>Manual Match
-Lender Amount: 58108.00
-Borrower Amount: 58108.00</t>
-        </is>
-      </c>
-      <c r="C110" s="9" t="inlineStr"/>
-      <c r="D110" s="9" t="inlineStr"/>
-      <c r="E110" s="15" t="inlineStr">
+      <c r="A110" s="1" t="inlineStr"/>
+      <c r="B110" s="2" t="inlineStr">
+        <is>
+          <t>No match found - No matching criteria met</t>
+        </is>
+      </c>
+      <c r="C110" s="1" t="inlineStr"/>
+      <c r="D110" s="1" t="inlineStr"/>
+      <c r="E110" s="26" t="inlineStr">
         <is>
           <t>Amount paid as interunit vendor payment.(Pragati Life Insurance Limited)</t>
         </is>
       </c>
-      <c r="F110" s="9" t="inlineStr"/>
-      <c r="G110" s="9" t="inlineStr"/>
-      <c r="H110" s="9" t="inlineStr"/>
-      <c r="I110" s="9" t="inlineStr"/>
-      <c r="J110" s="9" t="inlineStr"/>
-      <c r="K110" s="9" t="inlineStr"/>
-      <c r="L110" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F110" s="1" t="inlineStr"/>
+      <c r="G110" s="1" t="inlineStr"/>
+      <c r="H110" s="1" t="inlineStr"/>
+      <c r="I110" s="1" t="inlineStr"/>
+      <c r="J110" s="1" t="inlineStr"/>
+      <c r="K110" s="1" t="inlineStr"/>
+      <c r="L110" s="1" t="inlineStr"/>
     </row>
     <row r="111">
-      <c r="A111" s="9" t="inlineStr">
-        <is>
-          <t>M056</t>
-        </is>
-      </c>
-      <c r="B111" s="10" t="inlineStr"/>
-      <c r="C111" s="9" t="inlineStr"/>
-      <c r="D111" s="9" t="inlineStr">
+      <c r="A111" s="1" t="inlineStr"/>
+      <c r="B111" s="2" t="inlineStr"/>
+      <c r="C111" s="1" t="inlineStr"/>
+      <c r="D111" s="1" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E111" s="16" t="inlineStr">
+      <c r="E111" s="27" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F111" s="9" t="inlineStr"/>
-      <c r="G111" s="9" t="inlineStr"/>
-      <c r="H111" s="9" t="inlineStr"/>
-      <c r="I111" s="9" t="inlineStr"/>
-      <c r="J111" s="9" t="inlineStr"/>
-      <c r="K111" s="9" t="inlineStr"/>
-      <c r="L111" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F111" s="1" t="inlineStr"/>
+      <c r="G111" s="1" t="inlineStr"/>
+      <c r="H111" s="1" t="inlineStr"/>
+      <c r="I111" s="1" t="inlineStr"/>
+      <c r="J111" s="1" t="inlineStr"/>
+      <c r="K111" s="1" t="inlineStr"/>
+      <c r="L111" s="1" t="inlineStr"/>
     </row>
     <row r="112">
-      <c r="A112" s="17" t="inlineStr">
-        <is>
-          <t>M057</t>
-        </is>
-      </c>
-      <c r="B112" s="18" t="inlineStr"/>
-      <c r="C112" s="19" t="inlineStr">
+      <c r="A112" s="1" t="inlineStr"/>
+      <c r="B112" s="2" t="inlineStr"/>
+      <c r="C112" s="6" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D112" s="17" t="inlineStr">
+      <c r="D112" s="1" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E112" s="20" t="inlineStr">
+      <c r="E112" s="7" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F112" s="17" t="inlineStr"/>
-      <c r="G112" s="17" t="inlineStr"/>
-      <c r="H112" s="21" t="inlineStr">
+      <c r="F112" s="1" t="inlineStr"/>
+      <c r="G112" s="1" t="inlineStr"/>
+      <c r="H112" s="25" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I112" s="17" t="inlineStr">
+      <c r="I112" s="1" t="inlineStr">
         <is>
           <t>70715</t>
         </is>
       </c>
-      <c r="J112" s="22" t="inlineStr">
+      <c r="J112" s="8" t="inlineStr">
         <is>
           <t>11535</t>
         </is>
       </c>
-      <c r="K112" s="17" t="inlineStr"/>
-      <c r="L112" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="K112" s="1" t="inlineStr"/>
+      <c r="L112" s="1" t="inlineStr"/>
     </row>
     <row r="113">
-      <c r="A113" s="17" t="inlineStr">
-        <is>
-          <t>M057</t>
-        </is>
-      </c>
-      <c r="B113" s="18" t="inlineStr">
-        <is>
-          <t>Manual Match
-Lender Amount: 11535.00
-Borrower Amount: 11535.00</t>
-        </is>
-      </c>
-      <c r="C113" s="17" t="inlineStr"/>
-      <c r="D113" s="17" t="inlineStr"/>
-      <c r="E113" s="23" t="inlineStr">
+      <c r="A113" s="1" t="inlineStr"/>
+      <c r="B113" s="2" t="inlineStr">
+        <is>
+          <t>No match found - No matching criteria met</t>
+        </is>
+      </c>
+      <c r="C113" s="1" t="inlineStr"/>
+      <c r="D113" s="1" t="inlineStr"/>
+      <c r="E113" s="26" t="inlineStr">
         <is>
           <t>Amount paid as interunit vendor payment.(ARK Fire Fighting Manufacture Co.)</t>
         </is>
       </c>
-      <c r="F113" s="17" t="inlineStr"/>
-      <c r="G113" s="17" t="inlineStr"/>
-      <c r="H113" s="17" t="inlineStr"/>
-      <c r="I113" s="17" t="inlineStr"/>
-      <c r="J113" s="17" t="inlineStr"/>
-      <c r="K113" s="17" t="inlineStr"/>
-      <c r="L113" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F113" s="1" t="inlineStr"/>
+      <c r="G113" s="1" t="inlineStr"/>
+      <c r="H113" s="1" t="inlineStr"/>
+      <c r="I113" s="1" t="inlineStr"/>
+      <c r="J113" s="1" t="inlineStr"/>
+      <c r="K113" s="1" t="inlineStr"/>
+      <c r="L113" s="1" t="inlineStr"/>
     </row>
     <row r="114">
-      <c r="A114" s="17" t="inlineStr">
-        <is>
-          <t>M057</t>
-        </is>
-      </c>
-      <c r="B114" s="18" t="inlineStr"/>
-      <c r="C114" s="17" t="inlineStr"/>
-      <c r="D114" s="17" t="inlineStr">
+      <c r="A114" s="1" t="inlineStr"/>
+      <c r="B114" s="2" t="inlineStr"/>
+      <c r="C114" s="1" t="inlineStr"/>
+      <c r="D114" s="1" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E114" s="24" t="inlineStr">
+      <c r="E114" s="27" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F114" s="17" t="inlineStr"/>
-      <c r="G114" s="17" t="inlineStr"/>
-      <c r="H114" s="17" t="inlineStr"/>
-      <c r="I114" s="17" t="inlineStr"/>
-      <c r="J114" s="17" t="inlineStr"/>
-      <c r="K114" s="17" t="inlineStr"/>
-      <c r="L114" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F114" s="1" t="inlineStr"/>
+      <c r="G114" s="1" t="inlineStr"/>
+      <c r="H114" s="1" t="inlineStr"/>
+      <c r="I114" s="1" t="inlineStr"/>
+      <c r="J114" s="1" t="inlineStr"/>
+      <c r="K114" s="1" t="inlineStr"/>
+      <c r="L114" s="1" t="inlineStr"/>
     </row>
     <row r="115">
-      <c r="A115" s="9" t="inlineStr">
-        <is>
-          <t>M058</t>
-        </is>
-      </c>
-      <c r="B115" s="10" t="inlineStr"/>
-      <c r="C115" s="11" t="inlineStr">
+      <c r="A115" s="1" t="inlineStr"/>
+      <c r="B115" s="2" t="inlineStr"/>
+      <c r="C115" s="6" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D115" s="9" t="inlineStr">
+      <c r="D115" s="1" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E115" s="12" t="inlineStr">
+      <c r="E115" s="7" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F115" s="9" t="inlineStr"/>
-      <c r="G115" s="9" t="inlineStr"/>
-      <c r="H115" s="13" t="inlineStr">
+      <c r="F115" s="1" t="inlineStr"/>
+      <c r="G115" s="1" t="inlineStr"/>
+      <c r="H115" s="25" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I115" s="9" t="inlineStr">
+      <c r="I115" s="1" t="inlineStr">
         <is>
           <t>70716</t>
         </is>
       </c>
-      <c r="J115" s="14" t="inlineStr">
+      <c r="J115" s="8" t="inlineStr">
         <is>
           <t>1344000</t>
         </is>
       </c>
-      <c r="K115" s="9" t="inlineStr"/>
-      <c r="L115" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="K115" s="1" t="inlineStr"/>
+      <c r="L115" s="1" t="inlineStr"/>
     </row>
     <row r="116">
-      <c r="A116" s="9" t="inlineStr">
-        <is>
-          <t>M058</t>
-        </is>
-      </c>
-      <c r="B116" s="10" t="inlineStr">
-        <is>
-          <t>Manual Match
-Lender Amount: 1344000.00
-Borrower Amount: 1344000.00</t>
-        </is>
-      </c>
-      <c r="C116" s="9" t="inlineStr"/>
-      <c r="D116" s="9" t="inlineStr"/>
-      <c r="E116" s="15" t="inlineStr">
+      <c r="A116" s="1" t="inlineStr"/>
+      <c r="B116" s="2" t="inlineStr">
+        <is>
+          <t>No match found - No matching criteria met</t>
+        </is>
+      </c>
+      <c r="C116" s="1" t="inlineStr"/>
+      <c r="D116" s="1" t="inlineStr"/>
+      <c r="E116" s="26" t="inlineStr">
         <is>
           <t>Amount paid as interunit vendor payment.(Rangpur Metal Industries Ltd.)</t>
         </is>
       </c>
-      <c r="F116" s="9" t="inlineStr"/>
-      <c r="G116" s="9" t="inlineStr"/>
-      <c r="H116" s="9" t="inlineStr"/>
-      <c r="I116" s="9" t="inlineStr"/>
-      <c r="J116" s="9" t="inlineStr"/>
-      <c r="K116" s="9" t="inlineStr"/>
-      <c r="L116" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F116" s="1" t="inlineStr"/>
+      <c r="G116" s="1" t="inlineStr"/>
+      <c r="H116" s="1" t="inlineStr"/>
+      <c r="I116" s="1" t="inlineStr"/>
+      <c r="J116" s="1" t="inlineStr"/>
+      <c r="K116" s="1" t="inlineStr"/>
+      <c r="L116" s="1" t="inlineStr"/>
     </row>
     <row r="117">
-      <c r="A117" s="9" t="inlineStr">
-        <is>
-          <t>M058</t>
-        </is>
-      </c>
-      <c r="B117" s="10" t="inlineStr"/>
-      <c r="C117" s="9" t="inlineStr"/>
-      <c r="D117" s="9" t="inlineStr">
+      <c r="A117" s="1" t="inlineStr"/>
+      <c r="B117" s="2" t="inlineStr"/>
+      <c r="C117" s="1" t="inlineStr"/>
+      <c r="D117" s="1" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E117" s="16" t="inlineStr">
+      <c r="E117" s="27" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F117" s="9" t="inlineStr"/>
-      <c r="G117" s="9" t="inlineStr"/>
-      <c r="H117" s="9" t="inlineStr"/>
-      <c r="I117" s="9" t="inlineStr"/>
-      <c r="J117" s="9" t="inlineStr"/>
-      <c r="K117" s="9" t="inlineStr"/>
-      <c r="L117" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F117" s="1" t="inlineStr"/>
+      <c r="G117" s="1" t="inlineStr"/>
+      <c r="H117" s="1" t="inlineStr"/>
+      <c r="I117" s="1" t="inlineStr"/>
+      <c r="J117" s="1" t="inlineStr"/>
+      <c r="K117" s="1" t="inlineStr"/>
+      <c r="L117" s="1" t="inlineStr"/>
     </row>
     <row r="118">
-      <c r="A118" s="17" t="inlineStr">
-        <is>
-          <t>M059</t>
-        </is>
-      </c>
-      <c r="B118" s="18" t="inlineStr"/>
-      <c r="C118" s="19" t="inlineStr">
+      <c r="A118" s="1" t="inlineStr"/>
+      <c r="B118" s="2" t="inlineStr"/>
+      <c r="C118" s="6" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D118" s="17" t="inlineStr">
+      <c r="D118" s="1" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E118" s="20" t="inlineStr">
+      <c r="E118" s="7" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F118" s="17" t="inlineStr"/>
-      <c r="G118" s="17" t="inlineStr"/>
-      <c r="H118" s="21" t="inlineStr">
+      <c r="F118" s="1" t="inlineStr"/>
+      <c r="G118" s="1" t="inlineStr"/>
+      <c r="H118" s="25" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I118" s="17" t="inlineStr">
+      <c r="I118" s="1" t="inlineStr">
         <is>
           <t>70717</t>
         </is>
       </c>
-      <c r="J118" s="22" t="inlineStr">
+      <c r="J118" s="8" t="inlineStr">
         <is>
           <t>3457391</t>
         </is>
       </c>
-      <c r="K118" s="17" t="inlineStr"/>
-      <c r="L118" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="K118" s="1" t="inlineStr"/>
+      <c r="L118" s="1" t="inlineStr"/>
     </row>
     <row r="119">
-      <c r="A119" s="17" t="inlineStr">
-        <is>
-          <t>M059</t>
-        </is>
-      </c>
-      <c r="B119" s="18" t="inlineStr">
-        <is>
-          <t>Manual Match
-Lender Amount: 3457391.00
-Borrower Amount: 3457391.00</t>
-        </is>
-      </c>
-      <c r="C119" s="17" t="inlineStr"/>
-      <c r="D119" s="17" t="inlineStr"/>
-      <c r="E119" s="23" t="inlineStr">
+      <c r="A119" s="1" t="inlineStr"/>
+      <c r="B119" s="2" t="inlineStr">
+        <is>
+          <t>No match found - No matching criteria met</t>
+        </is>
+      </c>
+      <c r="C119" s="1" t="inlineStr"/>
+      <c r="D119" s="1" t="inlineStr"/>
+      <c r="E119" s="26" t="inlineStr">
         <is>
           <t>Amount paid as interunit vendor payment.(Rangpur Metal Industries Ltd.)</t>
         </is>
       </c>
-      <c r="F119" s="17" t="inlineStr"/>
-      <c r="G119" s="17" t="inlineStr"/>
-      <c r="H119" s="17" t="inlineStr"/>
-      <c r="I119" s="17" t="inlineStr"/>
-      <c r="J119" s="17" t="inlineStr"/>
-      <c r="K119" s="17" t="inlineStr"/>
-      <c r="L119" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F119" s="1" t="inlineStr"/>
+      <c r="G119" s="1" t="inlineStr"/>
+      <c r="H119" s="1" t="inlineStr"/>
+      <c r="I119" s="1" t="inlineStr"/>
+      <c r="J119" s="1" t="inlineStr"/>
+      <c r="K119" s="1" t="inlineStr"/>
+      <c r="L119" s="1" t="inlineStr"/>
     </row>
     <row r="120">
-      <c r="A120" s="17" t="inlineStr">
-        <is>
-          <t>M059</t>
-        </is>
-      </c>
-      <c r="B120" s="18" t="inlineStr"/>
-      <c r="C120" s="17" t="inlineStr"/>
-      <c r="D120" s="17" t="inlineStr">
+      <c r="A120" s="1" t="inlineStr"/>
+      <c r="B120" s="2" t="inlineStr"/>
+      <c r="C120" s="1" t="inlineStr"/>
+      <c r="D120" s="1" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E120" s="24" t="inlineStr">
+      <c r="E120" s="27" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F120" s="17" t="inlineStr"/>
-      <c r="G120" s="17" t="inlineStr"/>
-      <c r="H120" s="17" t="inlineStr"/>
-      <c r="I120" s="17" t="inlineStr"/>
-      <c r="J120" s="17" t="inlineStr"/>
-      <c r="K120" s="17" t="inlineStr"/>
-      <c r="L120" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F120" s="1" t="inlineStr"/>
+      <c r="G120" s="1" t="inlineStr"/>
+      <c r="H120" s="1" t="inlineStr"/>
+      <c r="I120" s="1" t="inlineStr"/>
+      <c r="J120" s="1" t="inlineStr"/>
+      <c r="K120" s="1" t="inlineStr"/>
+      <c r="L120" s="1" t="inlineStr"/>
     </row>
     <row r="121">
-      <c r="A121" s="9" t="inlineStr">
-        <is>
-          <t>M060</t>
-        </is>
-      </c>
-      <c r="B121" s="10" t="inlineStr"/>
-      <c r="C121" s="11" t="inlineStr">
+      <c r="A121" s="1" t="inlineStr"/>
+      <c r="B121" s="2" t="inlineStr"/>
+      <c r="C121" s="6" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D121" s="9" t="inlineStr">
+      <c r="D121" s="1" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E121" s="12" t="inlineStr">
+      <c r="E121" s="7" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F121" s="9" t="inlineStr"/>
-      <c r="G121" s="9" t="inlineStr"/>
-      <c r="H121" s="13" t="inlineStr">
+      <c r="F121" s="1" t="inlineStr"/>
+      <c r="G121" s="1" t="inlineStr"/>
+      <c r="H121" s="25" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I121" s="9" t="inlineStr">
+      <c r="I121" s="1" t="inlineStr">
         <is>
           <t>70718</t>
         </is>
       </c>
-      <c r="J121" s="14" t="inlineStr">
+      <c r="J121" s="8" t="inlineStr">
         <is>
           <t>1234</t>
         </is>
       </c>
-      <c r="K121" s="9" t="inlineStr"/>
-      <c r="L121" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="K121" s="1" t="inlineStr"/>
+      <c r="L121" s="1" t="inlineStr"/>
     </row>
     <row r="122">
-      <c r="A122" s="9" t="inlineStr">
-        <is>
-          <t>M060</t>
-        </is>
-      </c>
-      <c r="B122" s="10" t="inlineStr">
-        <is>
-          <t>Manual Match
-Lender Amount: 1234.00
-Borrower Amount: 1234.00</t>
-        </is>
-      </c>
-      <c r="C122" s="9" t="inlineStr"/>
-      <c r="D122" s="9" t="inlineStr"/>
-      <c r="E122" s="15" t="inlineStr">
+      <c r="A122" s="1" t="inlineStr"/>
+      <c r="B122" s="2" t="inlineStr">
+        <is>
+          <t>No match found - No matching criteria met</t>
+        </is>
+      </c>
+      <c r="C122" s="1" t="inlineStr"/>
+      <c r="D122" s="1" t="inlineStr"/>
+      <c r="E122" s="26" t="inlineStr">
         <is>
           <t>Amount paid as interunit vendor payment.(Wintel Limited)</t>
         </is>
       </c>
-      <c r="F122" s="9" t="inlineStr"/>
-      <c r="G122" s="9" t="inlineStr"/>
-      <c r="H122" s="9" t="inlineStr"/>
-      <c r="I122" s="9" t="inlineStr"/>
-      <c r="J122" s="9" t="inlineStr"/>
-      <c r="K122" s="9" t="inlineStr"/>
-      <c r="L122" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F122" s="1" t="inlineStr"/>
+      <c r="G122" s="1" t="inlineStr"/>
+      <c r="H122" s="1" t="inlineStr"/>
+      <c r="I122" s="1" t="inlineStr"/>
+      <c r="J122" s="1" t="inlineStr"/>
+      <c r="K122" s="1" t="inlineStr"/>
+      <c r="L122" s="1" t="inlineStr"/>
     </row>
     <row r="123">
-      <c r="A123" s="9" t="inlineStr">
-        <is>
-          <t>M060</t>
-        </is>
-      </c>
-      <c r="B123" s="10" t="inlineStr"/>
-      <c r="C123" s="9" t="inlineStr"/>
-      <c r="D123" s="9" t="inlineStr">
+      <c r="A123" s="1" t="inlineStr"/>
+      <c r="B123" s="2" t="inlineStr"/>
+      <c r="C123" s="1" t="inlineStr"/>
+      <c r="D123" s="1" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E123" s="16" t="inlineStr">
+      <c r="E123" s="27" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F123" s="9" t="inlineStr"/>
-      <c r="G123" s="9" t="inlineStr"/>
-      <c r="H123" s="9" t="inlineStr"/>
-      <c r="I123" s="9" t="inlineStr"/>
-      <c r="J123" s="9" t="inlineStr"/>
-      <c r="K123" s="9" t="inlineStr"/>
-      <c r="L123" s="9" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F123" s="1" t="inlineStr"/>
+      <c r="G123" s="1" t="inlineStr"/>
+      <c r="H123" s="1" t="inlineStr"/>
+      <c r="I123" s="1" t="inlineStr"/>
+      <c r="J123" s="1" t="inlineStr"/>
+      <c r="K123" s="1" t="inlineStr"/>
+      <c r="L123" s="1" t="inlineStr"/>
     </row>
     <row r="124">
-      <c r="A124" s="17" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
-      <c r="B124" s="18" t="inlineStr"/>
-      <c r="C124" s="19" t="inlineStr">
+      <c r="A124" s="1" t="inlineStr"/>
+      <c r="B124" s="2" t="inlineStr"/>
+      <c r="C124" s="6" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D124" s="17" t="inlineStr">
+      <c r="D124" s="1" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E124" s="20" t="inlineStr">
+      <c r="E124" s="7" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F124" s="17" t="inlineStr"/>
-      <c r="G124" s="17" t="inlineStr"/>
-      <c r="H124" s="21" t="inlineStr">
+      <c r="F124" s="1" t="inlineStr"/>
+      <c r="G124" s="1" t="inlineStr"/>
+      <c r="H124" s="25" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I124" s="17" t="inlineStr">
+      <c r="I124" s="1" t="inlineStr">
         <is>
           <t>70719</t>
         </is>
       </c>
-      <c r="J124" s="22" t="inlineStr">
+      <c r="J124" s="8" t="inlineStr">
         <is>
           <t>200000</t>
         </is>
       </c>
-      <c r="K124" s="17" t="inlineStr"/>
-      <c r="L124" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="K124" s="1" t="inlineStr"/>
+      <c r="L124" s="1" t="inlineStr"/>
     </row>
     <row r="125">
-      <c r="A125" s="17" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
-      <c r="B125" s="18" t="inlineStr">
-        <is>
-          <t>Manual Match
-Lender Amount: 200000.00
-Borrower Amount: 200000.00</t>
-        </is>
-      </c>
-      <c r="C125" s="17" t="inlineStr"/>
-      <c r="D125" s="17" t="inlineStr"/>
-      <c r="E125" s="23" t="inlineStr">
+      <c r="A125" s="1" t="inlineStr"/>
+      <c r="B125" s="2" t="inlineStr">
+        <is>
+          <t>Unmatched Record
+Reasons:
+1. Borrower's narration does not contain lender's short code
+2. Settlement mismatch: File 1 IDs [], File 2 IDs ['92117']</t>
+        </is>
+      </c>
+      <c r="C125" s="1" t="inlineStr"/>
+      <c r="D125" s="1" t="inlineStr"/>
+      <c r="E125" s="26" t="inlineStr">
         <is>
           <t>Amount paid as interunit vendor payment.(A.B.M Anas Engineering)</t>
         </is>
       </c>
-      <c r="F125" s="17" t="inlineStr"/>
-      <c r="G125" s="17" t="inlineStr"/>
-      <c r="H125" s="17" t="inlineStr"/>
-      <c r="I125" s="17" t="inlineStr"/>
-      <c r="J125" s="17" t="inlineStr"/>
-      <c r="K125" s="17" t="inlineStr"/>
-      <c r="L125" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F125" s="1" t="inlineStr"/>
+      <c r="G125" s="1" t="inlineStr"/>
+      <c r="H125" s="1" t="inlineStr"/>
+      <c r="I125" s="1" t="inlineStr"/>
+      <c r="J125" s="1" t="inlineStr"/>
+      <c r="K125" s="1" t="inlineStr"/>
+      <c r="L125" s="1" t="inlineStr"/>
     </row>
     <row r="126">
-      <c r="A126" s="17" t="inlineStr">
-        <is>
-          <t>M061</t>
-        </is>
-      </c>
-      <c r="B126" s="18" t="inlineStr"/>
-      <c r="C126" s="17" t="inlineStr"/>
-      <c r="D126" s="17" t="inlineStr">
+      <c r="A126" s="1" t="inlineStr"/>
+      <c r="B126" s="2" t="inlineStr"/>
+      <c r="C126" s="1" t="inlineStr"/>
+      <c r="D126" s="1" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E126" s="24" t="inlineStr">
+      <c r="E126" s="27" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F126" s="17" t="inlineStr"/>
-      <c r="G126" s="17" t="inlineStr"/>
-      <c r="H126" s="17" t="inlineStr"/>
-      <c r="I126" s="17" t="inlineStr"/>
-      <c r="J126" s="17" t="inlineStr"/>
-      <c r="K126" s="17" t="inlineStr"/>
-      <c r="L126" s="17" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
+      <c r="F126" s="1" t="inlineStr"/>
+      <c r="G126" s="1" t="inlineStr"/>
+      <c r="H126" s="1" t="inlineStr"/>
+      <c r="I126" s="1" t="inlineStr"/>
+      <c r="J126" s="1" t="inlineStr"/>
+      <c r="K126" s="1" t="inlineStr"/>
+      <c r="L126" s="1" t="inlineStr"/>
     </row>
     <row r="127">
-      <c r="A127" s="9" t="inlineStr">
-        <is>
-          <t>M064</t>
-        </is>
-      </c>
-      <c r="B127" s="10" t="inlineStr"/>
-      <c r="C127" s="11" t="inlineStr">
+      <c r="A127" s="17" t="inlineStr">
+        <is>
+          <t>M053</t>
+        </is>
+      </c>
+      <c r="B127" s="18" t="inlineStr"/>
+      <c r="C127" s="19" t="inlineStr">
         <is>
           <t>04/Jun/2025</t>
         </is>
       </c>
-      <c r="D127" s="9" t="inlineStr">
+      <c r="D127" s="17" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E127" s="12" t="inlineStr">
+      <c r="E127" s="20" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F127" s="9" t="inlineStr"/>
-      <c r="G127" s="9" t="inlineStr"/>
-      <c r="H127" s="13" t="inlineStr">
+      <c r="F127" s="17" t="inlineStr"/>
+      <c r="G127" s="17" t="inlineStr"/>
+      <c r="H127" s="21" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I127" s="9" t="inlineStr">
+      <c r="I127" s="17" t="inlineStr">
         <is>
           <t>70720</t>
         </is>
       </c>
-      <c r="J127" s="14" t="inlineStr">
+      <c r="J127" s="22" t="inlineStr">
         <is>
           <t>36900</t>
         </is>
       </c>
-      <c r="K127" s="9" t="inlineStr"/>
-      <c r="L127" s="9" t="inlineStr">
+      <c r="K127" s="17" t="inlineStr"/>
+      <c r="L127" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="9" t="inlineStr">
-        <is>
-          <t>M064</t>
-        </is>
-      </c>
-      <c r="B128" s="10" t="inlineStr">
+      <c r="A128" s="17" t="inlineStr">
+        <is>
+          <t>M053</t>
+        </is>
+      </c>
+      <c r="B128" s="18" t="inlineStr">
         <is>
           <t>Manual Match
 Lender Amount: 36900.00
 Borrower Amount: 36900.00</t>
         </is>
       </c>
-      <c r="C128" s="9" t="inlineStr"/>
-      <c r="D128" s="9" t="inlineStr"/>
-      <c r="E128" s="15" t="inlineStr">
+      <c r="C128" s="17" t="inlineStr"/>
+      <c r="D128" s="17" t="inlineStr"/>
+      <c r="E128" s="23" t="inlineStr">
         <is>
           <t>Amount paid as interunit vendor payment.(A.B.M Anas Engineering)</t>
         </is>
       </c>
-      <c r="F128" s="9" t="inlineStr"/>
-      <c r="G128" s="9" t="inlineStr"/>
-      <c r="H128" s="9" t="inlineStr"/>
-      <c r="I128" s="9" t="inlineStr"/>
-      <c r="J128" s="9" t="inlineStr"/>
-      <c r="K128" s="9" t="inlineStr"/>
-      <c r="L128" s="9" t="inlineStr">
+      <c r="F128" s="17" t="inlineStr"/>
+      <c r="G128" s="17" t="inlineStr"/>
+      <c r="H128" s="17" t="inlineStr"/>
+      <c r="I128" s="17" t="inlineStr"/>
+      <c r="J128" s="17" t="inlineStr"/>
+      <c r="K128" s="17" t="inlineStr"/>
+      <c r="L128" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="9" t="inlineStr">
-        <is>
-          <t>M064</t>
-        </is>
-      </c>
-      <c r="B129" s="10" t="inlineStr"/>
-      <c r="C129" s="9" t="inlineStr"/>
-      <c r="D129" s="9" t="inlineStr">
+      <c r="A129" s="17" t="inlineStr">
+        <is>
+          <t>M053</t>
+        </is>
+      </c>
+      <c r="B129" s="18" t="inlineStr"/>
+      <c r="C129" s="17" t="inlineStr"/>
+      <c r="D129" s="17" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E129" s="16" t="inlineStr">
+      <c r="E129" s="24" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F129" s="9" t="inlineStr"/>
-      <c r="G129" s="9" t="inlineStr"/>
-      <c r="H129" s="9" t="inlineStr"/>
-      <c r="I129" s="9" t="inlineStr"/>
-      <c r="J129" s="9" t="inlineStr"/>
-      <c r="K129" s="9" t="inlineStr"/>
-      <c r="L129" s="9" t="inlineStr">
+      <c r="F129" s="17" t="inlineStr"/>
+      <c r="G129" s="17" t="inlineStr"/>
+      <c r="H129" s="17" t="inlineStr"/>
+      <c r="I129" s="17" t="inlineStr"/>
+      <c r="J129" s="17" t="inlineStr"/>
+      <c r="K129" s="17" t="inlineStr"/>
+      <c r="L129" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="17" t="inlineStr">
-        <is>
-          <t>M065</t>
-        </is>
-      </c>
-      <c r="B130" s="18" t="inlineStr"/>
-      <c r="C130" s="19" t="inlineStr">
+      <c r="A130" s="9" t="inlineStr">
+        <is>
+          <t>M054</t>
+        </is>
+      </c>
+      <c r="B130" s="10" t="inlineStr"/>
+      <c r="C130" s="11" t="inlineStr">
         <is>
           <t>18/Jun/2025</t>
         </is>
       </c>
-      <c r="D130" s="17" t="inlineStr">
+      <c r="D130" s="9" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E130" s="20" t="inlineStr">
+      <c r="E130" s="12" t="inlineStr">
         <is>
           <t>Mutual Trust Bank Ltd-(Hypo)-2411000001105</t>
         </is>
       </c>
-      <c r="F130" s="17" t="inlineStr"/>
-      <c r="G130" s="17" t="inlineStr"/>
-      <c r="H130" s="21" t="inlineStr">
+      <c r="F130" s="9" t="inlineStr"/>
+      <c r="G130" s="9" t="inlineStr"/>
+      <c r="H130" s="13" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I130" s="17" t="inlineStr">
+      <c r="I130" s="9" t="inlineStr">
         <is>
           <t>70688</t>
         </is>
       </c>
-      <c r="J130" s="22" t="inlineStr">
+      <c r="J130" s="14" t="inlineStr">
         <is>
           <t>1531483</t>
         </is>
       </c>
-      <c r="K130" s="17" t="inlineStr"/>
-      <c r="L130" s="17" t="inlineStr">
+      <c r="K130" s="9" t="inlineStr"/>
+      <c r="L130" s="9" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="17" t="inlineStr">
-        <is>
-          <t>M065</t>
-        </is>
-      </c>
-      <c r="B131" s="18" t="inlineStr">
+      <c r="A131" s="9" t="inlineStr">
+        <is>
+          <t>M054</t>
+        </is>
+      </c>
+      <c r="B131" s="10" t="inlineStr">
         <is>
           <t>Manual Match
 Lender Amount: 1531483.00
 Borrower Amount: 1531483.00</t>
         </is>
       </c>
-      <c r="C131" s="17" t="inlineStr"/>
-      <c r="D131" s="17" t="inlineStr"/>
-      <c r="E131" s="23" t="inlineStr">
+      <c r="C131" s="9" t="inlineStr"/>
+      <c r="D131" s="9" t="inlineStr"/>
+      <c r="E131" s="15" t="inlineStr">
         <is>
           <t>Amount paid as Inter Unit Loan A/C-Transformer Unit (Sadharan Bima Corporation)</t>
         </is>
       </c>
-      <c r="F131" s="17" t="inlineStr"/>
-      <c r="G131" s="17" t="inlineStr"/>
-      <c r="H131" s="17" t="inlineStr"/>
-      <c r="I131" s="17" t="inlineStr"/>
-      <c r="J131" s="17" t="inlineStr"/>
-      <c r="K131" s="17" t="inlineStr"/>
-      <c r="L131" s="17" t="inlineStr">
+      <c r="F131" s="9" t="inlineStr"/>
+      <c r="G131" s="9" t="inlineStr"/>
+      <c r="H131" s="9" t="inlineStr"/>
+      <c r="I131" s="9" t="inlineStr"/>
+      <c r="J131" s="9" t="inlineStr"/>
+      <c r="K131" s="9" t="inlineStr"/>
+      <c r="L131" s="9" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="17" t="inlineStr">
-        <is>
-          <t>M065</t>
-        </is>
-      </c>
-      <c r="B132" s="18" t="inlineStr"/>
-      <c r="C132" s="17" t="inlineStr"/>
-      <c r="D132" s="17" t="inlineStr">
+      <c r="A132" s="9" t="inlineStr">
+        <is>
+          <t>M054</t>
+        </is>
+      </c>
+      <c r="B132" s="10" t="inlineStr"/>
+      <c r="C132" s="9" t="inlineStr"/>
+      <c r="D132" s="9" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E132" s="24" t="inlineStr">
+      <c r="E132" s="16" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F132" s="17" t="inlineStr"/>
-      <c r="G132" s="17" t="inlineStr"/>
-      <c r="H132" s="17" t="inlineStr"/>
-      <c r="I132" s="17" t="inlineStr"/>
-      <c r="J132" s="17" t="inlineStr"/>
-      <c r="K132" s="17" t="inlineStr"/>
-      <c r="L132" s="17" t="inlineStr">
+      <c r="F132" s="9" t="inlineStr"/>
+      <c r="G132" s="9" t="inlineStr"/>
+      <c r="H132" s="9" t="inlineStr"/>
+      <c r="I132" s="9" t="inlineStr"/>
+      <c r="J132" s="9" t="inlineStr"/>
+      <c r="K132" s="9" t="inlineStr"/>
+      <c r="L132" s="9" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="9" t="inlineStr">
-        <is>
-          <t>M066</t>
-        </is>
-      </c>
-      <c r="B133" s="10" t="inlineStr"/>
-      <c r="C133" s="11" t="inlineStr">
+      <c r="A133" s="17" t="inlineStr">
+        <is>
+          <t>M055</t>
+        </is>
+      </c>
+      <c r="B133" s="18" t="inlineStr"/>
+      <c r="C133" s="19" t="inlineStr">
         <is>
           <t>18/Jun/2025</t>
         </is>
       </c>
-      <c r="D133" s="9" t="inlineStr">
+      <c r="D133" s="17" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E133" s="12" t="inlineStr">
+      <c r="E133" s="20" t="inlineStr">
         <is>
           <t>Mutual Trust Bank Ltd-(Hypo)-2411000001105</t>
         </is>
       </c>
-      <c r="F133" s="9" t="inlineStr"/>
-      <c r="G133" s="9" t="inlineStr"/>
-      <c r="H133" s="13" t="inlineStr">
+      <c r="F133" s="17" t="inlineStr"/>
+      <c r="G133" s="17" t="inlineStr"/>
+      <c r="H133" s="21" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I133" s="9" t="inlineStr">
+      <c r="I133" s="17" t="inlineStr">
         <is>
           <t>70689</t>
         </is>
       </c>
-      <c r="J133" s="14" t="inlineStr">
+      <c r="J133" s="22" t="inlineStr">
         <is>
           <t>589625</t>
         </is>
       </c>
-      <c r="K133" s="9" t="inlineStr"/>
-      <c r="L133" s="9" t="inlineStr">
+      <c r="K133" s="17" t="inlineStr"/>
+      <c r="L133" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="9" t="inlineStr">
-        <is>
-          <t>M066</t>
-        </is>
-      </c>
-      <c r="B134" s="10" t="inlineStr">
+      <c r="A134" s="17" t="inlineStr">
+        <is>
+          <t>M055</t>
+        </is>
+      </c>
+      <c r="B134" s="18" t="inlineStr">
         <is>
           <t>Manual Match
 Lender Amount: 589625.00
 Borrower Amount: 589625.00</t>
         </is>
       </c>
-      <c r="C134" s="9" t="inlineStr"/>
-      <c r="D134" s="9" t="inlineStr"/>
-      <c r="E134" s="15" t="inlineStr">
+      <c r="C134" s="17" t="inlineStr"/>
+      <c r="D134" s="17" t="inlineStr"/>
+      <c r="E134" s="23" t="inlineStr">
         <is>
           <t>Amount paid as Inter Unit Loan A/C-Transformer Unit (Narayanganj Palli Biddyut Samity-1)</t>
         </is>
       </c>
-      <c r="F134" s="9" t="inlineStr"/>
-      <c r="G134" s="9" t="inlineStr"/>
-      <c r="H134" s="9" t="inlineStr"/>
-      <c r="I134" s="9" t="inlineStr"/>
-      <c r="J134" s="9" t="inlineStr"/>
-      <c r="K134" s="9" t="inlineStr"/>
-      <c r="L134" s="9" t="inlineStr">
+      <c r="F134" s="17" t="inlineStr"/>
+      <c r="G134" s="17" t="inlineStr"/>
+      <c r="H134" s="17" t="inlineStr"/>
+      <c r="I134" s="17" t="inlineStr"/>
+      <c r="J134" s="17" t="inlineStr"/>
+      <c r="K134" s="17" t="inlineStr"/>
+      <c r="L134" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="9" t="inlineStr">
-        <is>
-          <t>M066</t>
-        </is>
-      </c>
-      <c r="B135" s="10" t="inlineStr"/>
-      <c r="C135" s="9" t="inlineStr"/>
-      <c r="D135" s="9" t="inlineStr">
+      <c r="A135" s="17" t="inlineStr">
+        <is>
+          <t>M055</t>
+        </is>
+      </c>
+      <c r="B135" s="18" t="inlineStr"/>
+      <c r="C135" s="17" t="inlineStr"/>
+      <c r="D135" s="17" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E135" s="16" t="inlineStr">
+      <c r="E135" s="24" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F135" s="9" t="inlineStr"/>
-      <c r="G135" s="9" t="inlineStr"/>
-      <c r="H135" s="9" t="inlineStr"/>
-      <c r="I135" s="9" t="inlineStr"/>
-      <c r="J135" s="9" t="inlineStr"/>
-      <c r="K135" s="9" t="inlineStr"/>
-      <c r="L135" s="9" t="inlineStr">
+      <c r="F135" s="17" t="inlineStr"/>
+      <c r="G135" s="17" t="inlineStr"/>
+      <c r="H135" s="17" t="inlineStr"/>
+      <c r="I135" s="17" t="inlineStr"/>
+      <c r="J135" s="17" t="inlineStr"/>
+      <c r="K135" s="17" t="inlineStr"/>
+      <c r="L135" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="17" t="inlineStr">
+      <c r="A136" s="9" t="inlineStr">
         <is>
           <t>M005</t>
         </is>
       </c>
-      <c r="B136" s="18" t="inlineStr"/>
-      <c r="C136" s="19" t="inlineStr">
+      <c r="B136" s="10" t="inlineStr"/>
+      <c r="C136" s="11" t="inlineStr">
         <is>
           <t>21/Jun/2025</t>
         </is>
       </c>
-      <c r="D136" s="17" t="inlineStr">
+      <c r="D136" s="9" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E136" s="20" t="inlineStr">
+      <c r="E136" s="12" t="inlineStr">
         <is>
           <t>(as per details)</t>
         </is>
       </c>
-      <c r="F136" s="17" t="inlineStr"/>
-      <c r="G136" s="17" t="inlineStr"/>
-      <c r="H136" s="21" t="inlineStr">
+      <c r="F136" s="9" t="inlineStr"/>
+      <c r="G136" s="9" t="inlineStr"/>
+      <c r="H136" s="13" t="inlineStr">
         <is>
           <t>Journal</t>
         </is>
       </c>
-      <c r="I136" s="17" t="inlineStr">
+      <c r="I136" s="9" t="inlineStr">
         <is>
           <t>3538</t>
         </is>
       </c>
-      <c r="J136" s="22" t="inlineStr">
+      <c r="J136" s="14" t="inlineStr">
         <is>
           <t>200000</t>
         </is>
       </c>
-      <c r="K136" s="17" t="inlineStr"/>
-      <c r="L136" s="17" t="inlineStr">
+      <c r="K136" s="9" t="inlineStr"/>
+      <c r="L136" s="9" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="17" t="inlineStr">
+      <c r="A137" s="9" t="inlineStr">
         <is>
           <t>M005</t>
         </is>
       </c>
-      <c r="B137" s="18" t="inlineStr"/>
-      <c r="C137" s="17" t="inlineStr"/>
-      <c r="D137" s="17" t="inlineStr"/>
-      <c r="E137" s="20" t="inlineStr">
+      <c r="B137" s="10" t="inlineStr"/>
+      <c r="C137" s="9" t="inlineStr"/>
+      <c r="D137" s="9" t="inlineStr"/>
+      <c r="E137" s="12" t="inlineStr">
         <is>
           <t>Inter Unit Loan A/C-Pole Unit</t>
         </is>
       </c>
-      <c r="F137" s="17" t="inlineStr"/>
-      <c r="G137" s="17" t="inlineStr"/>
-      <c r="H137" s="17" t="inlineStr"/>
-      <c r="I137" s="17" t="inlineStr"/>
-      <c r="J137" s="22" t="inlineStr">
+      <c r="F137" s="9" t="inlineStr"/>
+      <c r="G137" s="9" t="inlineStr"/>
+      <c r="H137" s="9" t="inlineStr"/>
+      <c r="I137" s="9" t="inlineStr"/>
+      <c r="J137" s="14" t="inlineStr">
         <is>
           <t>200000</t>
         </is>
       </c>
-      <c r="K137" s="17" t="inlineStr"/>
-      <c r="L137" s="17" t="inlineStr">
+      <c r="K137" s="9" t="inlineStr"/>
+      <c r="L137" s="9" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="17" t="inlineStr">
+      <c r="A138" s="9" t="inlineStr">
         <is>
           <t>M005</t>
         </is>
       </c>
-      <c r="B138" s="18" t="inlineStr"/>
-      <c r="C138" s="17" t="inlineStr"/>
-      <c r="D138" s="17" t="inlineStr"/>
-      <c r="E138" s="20" t="inlineStr">
+      <c r="B138" s="10" t="inlineStr"/>
+      <c r="C138" s="9" t="inlineStr"/>
+      <c r="D138" s="9" t="inlineStr"/>
+      <c r="E138" s="12" t="inlineStr">
         <is>
           <t>Adv-Odoo Bangladesh</t>
         </is>
       </c>
-      <c r="F138" s="17" t="inlineStr"/>
-      <c r="G138" s="17" t="inlineStr"/>
-      <c r="H138" s="17" t="inlineStr"/>
-      <c r="I138" s="17" t="inlineStr"/>
-      <c r="J138" s="17" t="inlineStr"/>
-      <c r="K138" s="22" t="inlineStr">
+      <c r="F138" s="9" t="inlineStr"/>
+      <c r="G138" s="9" t="inlineStr"/>
+      <c r="H138" s="9" t="inlineStr"/>
+      <c r="I138" s="9" t="inlineStr"/>
+      <c r="J138" s="9" t="inlineStr"/>
+      <c r="K138" s="14" t="inlineStr">
         <is>
           <t>400000</t>
         </is>
       </c>
-      <c r="L138" s="17" t="inlineStr">
+      <c r="L138" s="9" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="17" t="inlineStr">
+      <c r="A139" s="9" t="inlineStr">
         <is>
           <t>M005</t>
         </is>
       </c>
-      <c r="B139" s="18" t="inlineStr">
+      <c r="B139" s="10" t="inlineStr">
         <is>
           <t>Narration Match
 Lender Amount: 200000.00
 Borrower Amount: 200000.00</t>
         </is>
       </c>
-      <c r="C139" s="17" t="inlineStr"/>
-      <c r="D139" s="17" t="inlineStr"/>
-      <c r="E139" s="23" t="inlineStr">
+      <c r="C139" s="9" t="inlineStr"/>
+      <c r="D139" s="9" t="inlineStr"/>
+      <c r="E139" s="15" t="inlineStr">
         <is>
           <t>Advance Chq no-8163057.  paid to Odoo Bangladesh agt ERP Emplemention. Ref no-IT/2014/11/008. from CIL Steel unit but 50% bill Tk.2,00,000 recorded in CIL-Trancformer and CIL-Pole Tk.2,00,000 So, Now made voucher as interunit loan.</t>
         </is>
       </c>
-      <c r="F139" s="17" t="inlineStr"/>
-      <c r="G139" s="17" t="inlineStr"/>
-      <c r="H139" s="17" t="inlineStr"/>
-      <c r="I139" s="17" t="inlineStr"/>
-      <c r="J139" s="17" t="inlineStr"/>
-      <c r="K139" s="17" t="inlineStr"/>
-      <c r="L139" s="17" t="inlineStr">
+      <c r="F139" s="9" t="inlineStr"/>
+      <c r="G139" s="9" t="inlineStr"/>
+      <c r="H139" s="9" t="inlineStr"/>
+      <c r="I139" s="9" t="inlineStr"/>
+      <c r="J139" s="9" t="inlineStr"/>
+      <c r="K139" s="9" t="inlineStr"/>
+      <c r="L139" s="9" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="17" t="inlineStr">
+      <c r="A140" s="9" t="inlineStr">
         <is>
           <t>M005</t>
         </is>
       </c>
-      <c r="B140" s="18" t="inlineStr"/>
-      <c r="C140" s="17" t="inlineStr"/>
-      <c r="D140" s="17" t="inlineStr">
+      <c r="B140" s="10" t="inlineStr"/>
+      <c r="C140" s="9" t="inlineStr"/>
+      <c r="D140" s="9" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E140" s="24" t="inlineStr">
+      <c r="E140" s="16" t="inlineStr">
         <is>
           <t>ziaul</t>
         </is>
       </c>
-      <c r="F140" s="17" t="inlineStr"/>
-      <c r="G140" s="17" t="inlineStr"/>
-      <c r="H140" s="17" t="inlineStr"/>
-      <c r="I140" s="17" t="inlineStr"/>
-      <c r="J140" s="17" t="inlineStr"/>
-      <c r="K140" s="17" t="inlineStr"/>
-      <c r="L140" s="17" t="inlineStr">
+      <c r="F140" s="9" t="inlineStr"/>
+      <c r="G140" s="9" t="inlineStr"/>
+      <c r="H140" s="9" t="inlineStr"/>
+      <c r="I140" s="9" t="inlineStr"/>
+      <c r="J140" s="9" t="inlineStr"/>
+      <c r="K140" s="9" t="inlineStr"/>
+      <c r="L140" s="9" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="9" t="inlineStr">
+      <c r="A141" s="17" t="inlineStr">
         <is>
           <t>M007</t>
         </is>
       </c>
-      <c r="B141" s="10" t="inlineStr"/>
-      <c r="C141" s="11" t="inlineStr">
+      <c r="B141" s="18" t="inlineStr"/>
+      <c r="C141" s="19" t="inlineStr">
         <is>
           <t>23/Jun/2025</t>
         </is>
       </c>
-      <c r="D141" s="9" t="inlineStr">
+      <c r="D141" s="17" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E141" s="12" t="inlineStr">
+      <c r="E141" s="20" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F141" s="9" t="inlineStr"/>
-      <c r="G141" s="9" t="inlineStr"/>
-      <c r="H141" s="13" t="inlineStr">
+      <c r="F141" s="17" t="inlineStr"/>
+      <c r="G141" s="17" t="inlineStr"/>
+      <c r="H141" s="21" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I141" s="9" t="inlineStr">
+      <c r="I141" s="17" t="inlineStr">
         <is>
           <t>70482</t>
         </is>
       </c>
-      <c r="J141" s="14" t="inlineStr">
+      <c r="J141" s="22" t="inlineStr">
         <is>
           <t>85000</t>
         </is>
       </c>
-      <c r="K141" s="9" t="inlineStr"/>
-      <c r="L141" s="9" t="inlineStr">
+      <c r="K141" s="17" t="inlineStr"/>
+      <c r="L141" s="17" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="9" t="inlineStr">
+      <c r="A142" s="17" t="inlineStr">
         <is>
           <t>M007</t>
         </is>
       </c>
-      <c r="B142" s="10" t="inlineStr">
+      <c r="B142" s="18" t="inlineStr">
         <is>
           <t>LC Match: LC-308524012043/24
 Lender Amount: 85000.00
 Borrower Amount: 85000.00</t>
         </is>
       </c>
-      <c r="C142" s="9" t="inlineStr"/>
-      <c r="D142" s="9" t="inlineStr"/>
-      <c r="E142" s="15" t="inlineStr">
+      <c r="C142" s="17" t="inlineStr"/>
+      <c r="D142" s="17" t="inlineStr"/>
+      <c r="E142" s="23" t="inlineStr">
         <is>
           <t>Amount being paid as Port,Shipping &amp; Carrying Charges agt LC-308524012043/24-Transformer Unit-[Item-OLTC-Project-PBSH-G-89-Team-A][C-1164524]</t>
         </is>
       </c>
-      <c r="F142" s="9" t="inlineStr"/>
-      <c r="G142" s="9" t="inlineStr"/>
-      <c r="H142" s="9" t="inlineStr"/>
-      <c r="I142" s="9" t="inlineStr"/>
-      <c r="J142" s="9" t="inlineStr"/>
-      <c r="K142" s="9" t="inlineStr"/>
-      <c r="L142" s="9" t="inlineStr">
+      <c r="F142" s="17" t="inlineStr"/>
+      <c r="G142" s="17" t="inlineStr"/>
+      <c r="H142" s="17" t="inlineStr"/>
+      <c r="I142" s="17" t="inlineStr"/>
+      <c r="J142" s="17" t="inlineStr"/>
+      <c r="K142" s="17" t="inlineStr"/>
+      <c r="L142" s="17" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="9" t="inlineStr">
+      <c r="A143" s="17" t="inlineStr">
         <is>
           <t>M007</t>
         </is>
       </c>
-      <c r="B143" s="10" t="inlineStr"/>
-      <c r="C143" s="9" t="inlineStr"/>
-      <c r="D143" s="9" t="inlineStr">
+      <c r="B143" s="18" t="inlineStr"/>
+      <c r="C143" s="17" t="inlineStr"/>
+      <c r="D143" s="17" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E143" s="16" t="inlineStr">
+      <c r="E143" s="24" t="inlineStr">
         <is>
           <t>shabbirul</t>
         </is>
       </c>
-      <c r="F143" s="9" t="inlineStr"/>
-      <c r="G143" s="9" t="inlineStr"/>
-      <c r="H143" s="9" t="inlineStr"/>
-      <c r="I143" s="9" t="inlineStr"/>
-      <c r="J143" s="9" t="inlineStr"/>
-      <c r="K143" s="9" t="inlineStr"/>
-      <c r="L143" s="9" t="inlineStr">
+      <c r="F143" s="17" t="inlineStr"/>
+      <c r="G143" s="17" t="inlineStr"/>
+      <c r="H143" s="17" t="inlineStr"/>
+      <c r="I143" s="17" t="inlineStr"/>
+      <c r="J143" s="17" t="inlineStr"/>
+      <c r="K143" s="17" t="inlineStr"/>
+      <c r="L143" s="17" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="17" t="inlineStr">
+      <c r="A144" s="9" t="inlineStr">
         <is>
           <t>M009</t>
         </is>
       </c>
-      <c r="B144" s="18" t="inlineStr"/>
-      <c r="C144" s="19" t="inlineStr">
+      <c r="B144" s="10" t="inlineStr"/>
+      <c r="C144" s="11" t="inlineStr">
         <is>
           <t>23/Jun/2025</t>
         </is>
       </c>
-      <c r="D144" s="17" t="inlineStr">
+      <c r="D144" s="9" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E144" s="20" t="inlineStr">
+      <c r="E144" s="12" t="inlineStr">
         <is>
           <t>Prime Bank-CD-2126117010855</t>
         </is>
       </c>
-      <c r="F144" s="17" t="inlineStr"/>
-      <c r="G144" s="17" t="inlineStr"/>
-      <c r="H144" s="21" t="inlineStr">
+      <c r="F144" s="9" t="inlineStr"/>
+      <c r="G144" s="9" t="inlineStr"/>
+      <c r="H144" s="13" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I144" s="17" t="inlineStr">
+      <c r="I144" s="9" t="inlineStr">
         <is>
           <t>70541</t>
         </is>
       </c>
-      <c r="J144" s="22" t="inlineStr">
+      <c r="J144" s="14" t="inlineStr">
         <is>
           <t>272808.31</t>
         </is>
       </c>
-      <c r="K144" s="17" t="inlineStr"/>
-      <c r="L144" s="17" t="inlineStr">
+      <c r="K144" s="9" t="inlineStr"/>
+      <c r="L144" s="9" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="17" t="inlineStr">
+      <c r="A145" s="9" t="inlineStr">
         <is>
           <t>M009</t>
         </is>
       </c>
-      <c r="B145" s="18" t="inlineStr">
+      <c r="B145" s="10" t="inlineStr">
         <is>
           <t>Narration Match
 Lender Amount: 272808.31
 Borrower Amount: 272808.31</t>
         </is>
       </c>
-      <c r="C145" s="17" t="inlineStr"/>
-      <c r="D145" s="17" t="inlineStr"/>
-      <c r="E145" s="23" t="inlineStr">
+      <c r="C145" s="9" t="inlineStr"/>
+      <c r="D145" s="9" t="inlineStr"/>
+      <c r="E145" s="15" t="inlineStr">
         <is>
           <t>Amount being paid as Principal &amp; Interest Repayment of Time Loan of Transformer-LD-2435445106</t>
         </is>
       </c>
-      <c r="F145" s="17" t="inlineStr"/>
-      <c r="G145" s="17" t="inlineStr"/>
-      <c r="H145" s="17" t="inlineStr"/>
-      <c r="I145" s="17" t="inlineStr"/>
-      <c r="J145" s="17" t="inlineStr"/>
-      <c r="K145" s="17" t="inlineStr"/>
-      <c r="L145" s="17" t="inlineStr">
+      <c r="F145" s="9" t="inlineStr"/>
+      <c r="G145" s="9" t="inlineStr"/>
+      <c r="H145" s="9" t="inlineStr"/>
+      <c r="I145" s="9" t="inlineStr"/>
+      <c r="J145" s="9" t="inlineStr"/>
+      <c r="K145" s="9" t="inlineStr"/>
+      <c r="L145" s="9" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="17" t="inlineStr">
+      <c r="A146" s="9" t="inlineStr">
         <is>
           <t>M009</t>
         </is>
       </c>
-      <c r="B146" s="18" t="inlineStr"/>
-      <c r="C146" s="17" t="inlineStr"/>
-      <c r="D146" s="17" t="inlineStr">
+      <c r="B146" s="10" t="inlineStr"/>
+      <c r="C146" s="9" t="inlineStr"/>
+      <c r="D146" s="9" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E146" s="24" t="inlineStr">
+      <c r="E146" s="16" t="inlineStr">
         <is>
           <t>shabbirul</t>
         </is>
       </c>
-      <c r="F146" s="17" t="inlineStr"/>
-      <c r="G146" s="17" t="inlineStr"/>
-      <c r="H146" s="17" t="inlineStr"/>
-      <c r="I146" s="17" t="inlineStr"/>
-      <c r="J146" s="17" t="inlineStr"/>
-      <c r="K146" s="17" t="inlineStr"/>
-      <c r="L146" s="17" t="inlineStr">
+      <c r="F146" s="9" t="inlineStr"/>
+      <c r="G146" s="9" t="inlineStr"/>
+      <c r="H146" s="9" t="inlineStr"/>
+      <c r="I146" s="9" t="inlineStr"/>
+      <c r="J146" s="9" t="inlineStr"/>
+      <c r="K146" s="9" t="inlineStr"/>
+      <c r="L146" s="9" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="9" t="inlineStr">
+      <c r="A147" s="17" t="inlineStr">
         <is>
           <t>M011</t>
         </is>
       </c>
-      <c r="B147" s="10" t="inlineStr"/>
-      <c r="C147" s="11" t="inlineStr">
+      <c r="B147" s="18" t="inlineStr"/>
+      <c r="C147" s="19" t="inlineStr">
         <is>
           <t>23/Jun/2025</t>
         </is>
       </c>
-      <c r="D147" s="9" t="inlineStr">
+      <c r="D147" s="17" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E147" s="12" t="inlineStr">
+      <c r="E147" s="20" t="inlineStr">
         <is>
           <t>Prime Bank-CD-2126117010855</t>
         </is>
       </c>
-      <c r="F147" s="9" t="inlineStr"/>
-      <c r="G147" s="9" t="inlineStr"/>
-      <c r="H147" s="13" t="inlineStr">
+      <c r="F147" s="17" t="inlineStr"/>
+      <c r="G147" s="17" t="inlineStr"/>
+      <c r="H147" s="21" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I147" s="9" t="inlineStr">
+      <c r="I147" s="17" t="inlineStr">
         <is>
           <t>70548</t>
         </is>
       </c>
-      <c r="J147" s="14" t="inlineStr">
+      <c r="J147" s="22" t="inlineStr">
         <is>
           <t>133619.23</t>
         </is>
       </c>
-      <c r="K147" s="9" t="inlineStr"/>
-      <c r="L147" s="9" t="inlineStr">
+      <c r="K147" s="17" t="inlineStr"/>
+      <c r="L147" s="17" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="9" t="inlineStr">
+      <c r="A148" s="17" t="inlineStr">
         <is>
           <t>M011</t>
         </is>
       </c>
-      <c r="B148" s="10" t="inlineStr">
+      <c r="B148" s="18" t="inlineStr">
         <is>
           <t>Narration Match
 Lender Amount: 133619.23
 Borrower Amount: 133619.23</t>
         </is>
       </c>
-      <c r="C148" s="9" t="inlineStr"/>
-      <c r="D148" s="9" t="inlineStr"/>
-      <c r="E148" s="15" t="inlineStr">
+      <c r="C148" s="17" t="inlineStr"/>
+      <c r="D148" s="17" t="inlineStr"/>
+      <c r="E148" s="23" t="inlineStr">
         <is>
           <t>Amount being paid as Principal &amp; Interest Repayment of Time Loan of Transformer-LD-2503002237</t>
         </is>
       </c>
-      <c r="F148" s="9" t="inlineStr"/>
-      <c r="G148" s="9" t="inlineStr"/>
-      <c r="H148" s="9" t="inlineStr"/>
-      <c r="I148" s="9" t="inlineStr"/>
-      <c r="J148" s="9" t="inlineStr"/>
-      <c r="K148" s="9" t="inlineStr"/>
-      <c r="L148" s="9" t="inlineStr">
+      <c r="F148" s="17" t="inlineStr"/>
+      <c r="G148" s="17" t="inlineStr"/>
+      <c r="H148" s="17" t="inlineStr"/>
+      <c r="I148" s="17" t="inlineStr"/>
+      <c r="J148" s="17" t="inlineStr"/>
+      <c r="K148" s="17" t="inlineStr"/>
+      <c r="L148" s="17" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="9" t="inlineStr">
+      <c r="A149" s="17" t="inlineStr">
         <is>
           <t>M011</t>
         </is>
       </c>
-      <c r="B149" s="10" t="inlineStr"/>
-      <c r="C149" s="9" t="inlineStr"/>
-      <c r="D149" s="9" t="inlineStr">
+      <c r="B149" s="18" t="inlineStr"/>
+      <c r="C149" s="17" t="inlineStr"/>
+      <c r="D149" s="17" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E149" s="16" t="inlineStr">
+      <c r="E149" s="24" t="inlineStr">
         <is>
           <t>shabbirul</t>
         </is>
       </c>
-      <c r="F149" s="9" t="inlineStr"/>
-      <c r="G149" s="9" t="inlineStr"/>
-      <c r="H149" s="9" t="inlineStr"/>
-      <c r="I149" s="9" t="inlineStr"/>
-      <c r="J149" s="9" t="inlineStr"/>
-      <c r="K149" s="9" t="inlineStr"/>
-      <c r="L149" s="9" t="inlineStr">
+      <c r="F149" s="17" t="inlineStr"/>
+      <c r="G149" s="17" t="inlineStr"/>
+      <c r="H149" s="17" t="inlineStr"/>
+      <c r="I149" s="17" t="inlineStr"/>
+      <c r="J149" s="17" t="inlineStr"/>
+      <c r="K149" s="17" t="inlineStr"/>
+      <c r="L149" s="17" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="17" t="inlineStr">
+      <c r="A150" s="9" t="inlineStr">
         <is>
           <t>M013</t>
         </is>
       </c>
-      <c r="B150" s="18" t="inlineStr"/>
-      <c r="C150" s="19" t="inlineStr">
+      <c r="B150" s="10" t="inlineStr"/>
+      <c r="C150" s="11" t="inlineStr">
         <is>
           <t>23/Jun/2025</t>
         </is>
       </c>
-      <c r="D150" s="17" t="inlineStr">
+      <c r="D150" s="9" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E150" s="20" t="inlineStr">
+      <c r="E150" s="12" t="inlineStr">
         <is>
           <t>Prime Bank-CD-2126117010855</t>
         </is>
       </c>
-      <c r="F150" s="17" t="inlineStr"/>
-      <c r="G150" s="17" t="inlineStr"/>
-      <c r="H150" s="21" t="inlineStr">
+      <c r="F150" s="9" t="inlineStr"/>
+      <c r="G150" s="9" t="inlineStr"/>
+      <c r="H150" s="13" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I150" s="17" t="inlineStr">
+      <c r="I150" s="9" t="inlineStr">
         <is>
           <t>70809</t>
         </is>
       </c>
-      <c r="J150" s="22" t="inlineStr">
+      <c r="J150" s="14" t="inlineStr">
         <is>
           <t>174172.7</t>
         </is>
       </c>
-      <c r="K150" s="17" t="inlineStr"/>
-      <c r="L150" s="17" t="inlineStr">
+      <c r="K150" s="9" t="inlineStr"/>
+      <c r="L150" s="9" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="17" t="inlineStr">
+      <c r="A151" s="9" t="inlineStr">
         <is>
           <t>M013</t>
         </is>
       </c>
-      <c r="B151" s="18" t="inlineStr">
+      <c r="B151" s="10" t="inlineStr">
         <is>
           <t>Narration Match
 Lender Amount: 174172.70
 Borrower Amount: 174172.70</t>
         </is>
       </c>
-      <c r="C151" s="17" t="inlineStr"/>
-      <c r="D151" s="17" t="inlineStr"/>
-      <c r="E151" s="23" t="inlineStr">
+      <c r="C151" s="9" t="inlineStr"/>
+      <c r="D151" s="9" t="inlineStr"/>
+      <c r="E151" s="15" t="inlineStr">
         <is>
           <t>Amount being paid as Principal &amp; Interest repayment of Time Loan-CIL Transformer-LD-2432680080</t>
         </is>
       </c>
-      <c r="F151" s="17" t="inlineStr"/>
-      <c r="G151" s="17" t="inlineStr"/>
-      <c r="H151" s="17" t="inlineStr"/>
-      <c r="I151" s="17" t="inlineStr"/>
-      <c r="J151" s="17" t="inlineStr"/>
-      <c r="K151" s="17" t="inlineStr"/>
-      <c r="L151" s="17" t="inlineStr">
+      <c r="F151" s="9" t="inlineStr"/>
+      <c r="G151" s="9" t="inlineStr"/>
+      <c r="H151" s="9" t="inlineStr"/>
+      <c r="I151" s="9" t="inlineStr"/>
+      <c r="J151" s="9" t="inlineStr"/>
+      <c r="K151" s="9" t="inlineStr"/>
+      <c r="L151" s="9" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="17" t="inlineStr">
+      <c r="A152" s="9" t="inlineStr">
         <is>
           <t>M013</t>
         </is>
       </c>
-      <c r="B152" s="18" t="inlineStr"/>
-      <c r="C152" s="17" t="inlineStr"/>
-      <c r="D152" s="17" t="inlineStr">
+      <c r="B152" s="10" t="inlineStr"/>
+      <c r="C152" s="9" t="inlineStr"/>
+      <c r="D152" s="9" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E152" s="24" t="inlineStr">
+      <c r="E152" s="16" t="inlineStr">
         <is>
           <t>shabbirul</t>
         </is>
       </c>
-      <c r="F152" s="17" t="inlineStr"/>
-      <c r="G152" s="17" t="inlineStr"/>
-      <c r="H152" s="17" t="inlineStr"/>
-      <c r="I152" s="17" t="inlineStr"/>
-      <c r="J152" s="17" t="inlineStr"/>
-      <c r="K152" s="17" t="inlineStr"/>
-      <c r="L152" s="17" t="inlineStr">
+      <c r="F152" s="9" t="inlineStr"/>
+      <c r="G152" s="9" t="inlineStr"/>
+      <c r="H152" s="9" t="inlineStr"/>
+      <c r="I152" s="9" t="inlineStr"/>
+      <c r="J152" s="9" t="inlineStr"/>
+      <c r="K152" s="9" t="inlineStr"/>
+      <c r="L152" s="9" t="inlineStr">
         <is>
           <t>Narration</t>
         </is>
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="9" t="inlineStr">
+      <c r="A153" s="17" t="inlineStr">
         <is>
           <t>M020</t>
         </is>
       </c>
-      <c r="B153" s="10" t="inlineStr"/>
-      <c r="C153" s="11" t="inlineStr">
+      <c r="B153" s="18" t="inlineStr"/>
+      <c r="C153" s="19" t="inlineStr">
         <is>
           <t>23/Jun/2025</t>
         </is>
       </c>
-      <c r="D153" s="9" t="inlineStr">
+      <c r="D153" s="17" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E153" s="12" t="inlineStr">
+      <c r="E153" s="20" t="inlineStr">
         <is>
           <t>Prime Bank-CD-2126117010855</t>
         </is>
       </c>
-      <c r="F153" s="9" t="inlineStr"/>
-      <c r="G153" s="9" t="inlineStr"/>
-      <c r="H153" s="13" t="inlineStr">
+      <c r="F153" s="17" t="inlineStr"/>
+      <c r="G153" s="17" t="inlineStr"/>
+      <c r="H153" s="21" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I153" s="9" t="inlineStr">
+      <c r="I153" s="17" t="inlineStr">
         <is>
           <t>70810</t>
         </is>
       </c>
-      <c r="J153" s="14" t="inlineStr">
+      <c r="J153" s="22" t="inlineStr">
         <is>
           <t>83197.81</t>
         </is>
       </c>
-      <c r="K153" s="9" t="inlineStr"/>
-      <c r="L153" s="9" t="inlineStr">
+      <c r="K153" s="17" t="inlineStr"/>
+      <c r="L153" s="17" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="9" t="inlineStr">
+      <c r="A154" s="17" t="inlineStr">
         <is>
           <t>M020</t>
         </is>
       </c>
-      <c r="B154" s="10" t="inlineStr">
+      <c r="B154" s="18" t="inlineStr">
         <is>
           <t>Interunit Loan Match: PBL#10855
 Lender Amount: 83197.81
 Borrower Amount: 83197.81</t>
         </is>
       </c>
-      <c r="C154" s="9" t="inlineStr"/>
-      <c r="D154" s="9" t="inlineStr"/>
-      <c r="E154" s="15" t="inlineStr">
+      <c r="C154" s="17" t="inlineStr"/>
+      <c r="D154" s="17" t="inlineStr"/>
+      <c r="E154" s="23" t="inlineStr">
         <is>
           <t>Amount being paid as Principal &amp; Interest Repayment of Time Loan of Transformer-LD-2502802705</t>
         </is>
       </c>
-      <c r="F154" s="9" t="inlineStr"/>
-      <c r="G154" s="9" t="inlineStr"/>
-      <c r="H154" s="9" t="inlineStr"/>
-      <c r="I154" s="9" t="inlineStr"/>
-      <c r="J154" s="9" t="inlineStr"/>
-      <c r="K154" s="9" t="inlineStr"/>
-      <c r="L154" s="9" t="inlineStr">
+      <c r="F154" s="17" t="inlineStr"/>
+      <c r="G154" s="17" t="inlineStr"/>
+      <c r="H154" s="17" t="inlineStr"/>
+      <c r="I154" s="17" t="inlineStr"/>
+      <c r="J154" s="17" t="inlineStr"/>
+      <c r="K154" s="17" t="inlineStr"/>
+      <c r="L154" s="17" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="9" t="inlineStr">
+      <c r="A155" s="17" t="inlineStr">
         <is>
           <t>M020</t>
         </is>
       </c>
-      <c r="B155" s="10" t="inlineStr"/>
-      <c r="C155" s="9" t="inlineStr"/>
-      <c r="D155" s="9" t="inlineStr">
+      <c r="B155" s="18" t="inlineStr"/>
+      <c r="C155" s="17" t="inlineStr"/>
+      <c r="D155" s="17" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E155" s="16" t="inlineStr">
+      <c r="E155" s="24" t="inlineStr">
         <is>
           <t>shabbirul</t>
         </is>
       </c>
-      <c r="F155" s="9" t="inlineStr"/>
-      <c r="G155" s="9" t="inlineStr"/>
-      <c r="H155" s="9" t="inlineStr"/>
-      <c r="I155" s="9" t="inlineStr"/>
-      <c r="J155" s="9" t="inlineStr"/>
-      <c r="K155" s="9" t="inlineStr"/>
-      <c r="L155" s="9" t="inlineStr">
+      <c r="F155" s="17" t="inlineStr"/>
+      <c r="G155" s="17" t="inlineStr"/>
+      <c r="H155" s="17" t="inlineStr"/>
+      <c r="I155" s="17" t="inlineStr"/>
+      <c r="J155" s="17" t="inlineStr"/>
+      <c r="K155" s="17" t="inlineStr"/>
+      <c r="L155" s="17" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="17" t="inlineStr">
+      <c r="A156" s="9" t="inlineStr">
         <is>
           <t>M021</t>
         </is>
       </c>
-      <c r="B156" s="18" t="inlineStr"/>
-      <c r="C156" s="19" t="inlineStr">
+      <c r="B156" s="10" t="inlineStr"/>
+      <c r="C156" s="11" t="inlineStr">
         <is>
           <t>25/Jun/2025</t>
         </is>
       </c>
-      <c r="D156" s="17" t="inlineStr">
+      <c r="D156" s="9" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E156" s="20" t="inlineStr">
+      <c r="E156" s="12" t="inlineStr">
         <is>
           <t>Eastern Bank,STD-1011220144056</t>
         </is>
       </c>
-      <c r="F156" s="17" t="inlineStr"/>
-      <c r="G156" s="17" t="inlineStr"/>
-      <c r="H156" s="21" t="inlineStr">
+      <c r="F156" s="9" t="inlineStr"/>
+      <c r="G156" s="9" t="inlineStr"/>
+      <c r="H156" s="13" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I156" s="17" t="inlineStr">
+      <c r="I156" s="9" t="inlineStr">
         <is>
           <t>70557</t>
         </is>
       </c>
-      <c r="J156" s="22" t="inlineStr">
+      <c r="J156" s="14" t="inlineStr">
         <is>
           <t>200000</t>
         </is>
       </c>
-      <c r="K156" s="17" t="inlineStr"/>
-      <c r="L156" s="17" t="inlineStr">
+      <c r="K156" s="9" t="inlineStr"/>
+      <c r="L156" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="17" t="inlineStr">
+      <c r="A157" s="9" t="inlineStr">
         <is>
           <t>M021</t>
         </is>
       </c>
-      <c r="B157" s="18" t="inlineStr">
+      <c r="B157" s="10" t="inlineStr">
         <is>
           <t>Interunit Loan Match: EBL#4056
 Lender Amount: 200000.00
 Borrower Amount: 200000.00</t>
         </is>
       </c>
-      <c r="C157" s="17" t="inlineStr"/>
-      <c r="D157" s="17" t="inlineStr"/>
-      <c r="E157" s="23" t="inlineStr">
+      <c r="C157" s="9" t="inlineStr"/>
+      <c r="D157" s="9" t="inlineStr"/>
+      <c r="E157" s="15" t="inlineStr">
         <is>
           <t>Interunit fund transfer as Inter Unit Loan A/C-Transformer Unit, EBL#44067</t>
         </is>
       </c>
-      <c r="F157" s="17" t="inlineStr"/>
-      <c r="G157" s="17" t="inlineStr"/>
-      <c r="H157" s="17" t="inlineStr"/>
-      <c r="I157" s="17" t="inlineStr"/>
-      <c r="J157" s="17" t="inlineStr"/>
-      <c r="K157" s="17" t="inlineStr"/>
-      <c r="L157" s="17" t="inlineStr">
+      <c r="F157" s="9" t="inlineStr"/>
+      <c r="G157" s="9" t="inlineStr"/>
+      <c r="H157" s="9" t="inlineStr"/>
+      <c r="I157" s="9" t="inlineStr"/>
+      <c r="J157" s="9" t="inlineStr"/>
+      <c r="K157" s="9" t="inlineStr"/>
+      <c r="L157" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="17" t="inlineStr">
+      <c r="A158" s="9" t="inlineStr">
         <is>
           <t>M021</t>
         </is>
       </c>
-      <c r="B158" s="18" t="inlineStr"/>
-      <c r="C158" s="17" t="inlineStr"/>
-      <c r="D158" s="17" t="inlineStr">
+      <c r="B158" s="10" t="inlineStr"/>
+      <c r="C158" s="9" t="inlineStr"/>
+      <c r="D158" s="9" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E158" s="24" t="inlineStr">
+      <c r="E158" s="16" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F158" s="17" t="inlineStr"/>
-      <c r="G158" s="17" t="inlineStr"/>
-      <c r="H158" s="17" t="inlineStr"/>
-      <c r="I158" s="17" t="inlineStr"/>
-      <c r="J158" s="17" t="inlineStr"/>
-      <c r="K158" s="17" t="inlineStr"/>
-      <c r="L158" s="17" t="inlineStr">
+      <c r="F158" s="9" t="inlineStr"/>
+      <c r="G158" s="9" t="inlineStr"/>
+      <c r="H158" s="9" t="inlineStr"/>
+      <c r="I158" s="9" t="inlineStr"/>
+      <c r="J158" s="9" t="inlineStr"/>
+      <c r="K158" s="9" t="inlineStr"/>
+      <c r="L158" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="9" t="inlineStr">
+      <c r="A159" s="17" t="inlineStr">
         <is>
           <t>M022</t>
         </is>
       </c>
-      <c r="B159" s="10" t="inlineStr"/>
-      <c r="C159" s="11" t="inlineStr">
+      <c r="B159" s="18" t="inlineStr"/>
+      <c r="C159" s="19" t="inlineStr">
         <is>
           <t>25/Jun/2025</t>
         </is>
       </c>
-      <c r="D159" s="9" t="inlineStr">
+      <c r="D159" s="17" t="inlineStr">
         <is>
           <t>Dr</t>
         </is>
       </c>
-      <c r="E159" s="12" t="inlineStr">
+      <c r="E159" s="20" t="inlineStr">
         <is>
           <t>Prime Bank-CD-2126117010855</t>
         </is>
       </c>
-      <c r="F159" s="9" t="inlineStr"/>
-      <c r="G159" s="9" t="inlineStr"/>
-      <c r="H159" s="13" t="inlineStr">
+      <c r="F159" s="17" t="inlineStr"/>
+      <c r="G159" s="17" t="inlineStr"/>
+      <c r="H159" s="21" t="inlineStr">
         <is>
           <t>Receipt</t>
         </is>
       </c>
-      <c r="I159" s="9" t="inlineStr">
+      <c r="I159" s="17" t="inlineStr">
         <is>
           <t>964</t>
         </is>
       </c>
-      <c r="J159" s="9" t="inlineStr"/>
-      <c r="K159" s="14" t="inlineStr">
+      <c r="J159" s="17" t="inlineStr"/>
+      <c r="K159" s="22" t="inlineStr">
         <is>
           <t>50000</t>
         </is>
       </c>
-      <c r="L159" s="9" t="inlineStr">
+      <c r="L159" s="17" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="9" t="inlineStr">
+      <c r="A160" s="17" t="inlineStr">
         <is>
           <t>M022</t>
         </is>
       </c>
-      <c r="B160" s="10" t="inlineStr">
+      <c r="B160" s="18" t="inlineStr">
         <is>
           <t>Interunit Loan Match: PBL#1060
 Lender Amount: 50000.00
 Borrower Amount: 50000.00</t>
         </is>
       </c>
-      <c r="C160" s="9" t="inlineStr"/>
-      <c r="D160" s="9" t="inlineStr"/>
-      <c r="E160" s="15" t="inlineStr">
+      <c r="C160" s="17" t="inlineStr"/>
+      <c r="D160" s="17" t="inlineStr"/>
+      <c r="E160" s="23" t="inlineStr">
         <is>
           <t>Interunit fund transfer as Inter Unit Loan A/C-Transformer Unit,PBL#1060</t>
         </is>
       </c>
-      <c r="F160" s="9" t="inlineStr"/>
-      <c r="G160" s="9" t="inlineStr"/>
-      <c r="H160" s="9" t="inlineStr"/>
-      <c r="I160" s="9" t="inlineStr"/>
-      <c r="J160" s="9" t="inlineStr"/>
-      <c r="K160" s="9" t="inlineStr"/>
-      <c r="L160" s="9" t="inlineStr">
+      <c r="F160" s="17" t="inlineStr"/>
+      <c r="G160" s="17" t="inlineStr"/>
+      <c r="H160" s="17" t="inlineStr"/>
+      <c r="I160" s="17" t="inlineStr"/>
+      <c r="J160" s="17" t="inlineStr"/>
+      <c r="K160" s="17" t="inlineStr"/>
+      <c r="L160" s="17" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="9" t="inlineStr">
+      <c r="A161" s="17" t="inlineStr">
         <is>
           <t>M022</t>
         </is>
       </c>
-      <c r="B161" s="10" t="inlineStr"/>
-      <c r="C161" s="9" t="inlineStr"/>
-      <c r="D161" s="9" t="inlineStr">
+      <c r="B161" s="18" t="inlineStr"/>
+      <c r="C161" s="17" t="inlineStr"/>
+      <c r="D161" s="17" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E161" s="16" t="inlineStr">
+      <c r="E161" s="24" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F161" s="9" t="inlineStr"/>
-      <c r="G161" s="9" t="inlineStr"/>
-      <c r="H161" s="9" t="inlineStr"/>
-      <c r="I161" s="9" t="inlineStr"/>
-      <c r="J161" s="9" t="inlineStr"/>
-      <c r="K161" s="9" t="inlineStr"/>
-      <c r="L161" s="9" t="inlineStr">
+      <c r="F161" s="17" t="inlineStr"/>
+      <c r="G161" s="17" t="inlineStr"/>
+      <c r="H161" s="17" t="inlineStr"/>
+      <c r="I161" s="17" t="inlineStr"/>
+      <c r="J161" s="17" t="inlineStr"/>
+      <c r="K161" s="17" t="inlineStr"/>
+      <c r="L161" s="17" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="17" t="inlineStr">
+      <c r="A162" s="9" t="inlineStr">
         <is>
           <t>M023</t>
         </is>
       </c>
-      <c r="B162" s="18" t="inlineStr"/>
-      <c r="C162" s="19" t="inlineStr">
+      <c r="B162" s="10" t="inlineStr"/>
+      <c r="C162" s="11" t="inlineStr">
         <is>
           <t>25/Jun/2025</t>
         </is>
       </c>
-      <c r="D162" s="17" t="inlineStr">
+      <c r="D162" s="9" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E162" s="20" t="inlineStr">
+      <c r="E162" s="12" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F162" s="17" t="inlineStr"/>
-      <c r="G162" s="17" t="inlineStr"/>
-      <c r="H162" s="21" t="inlineStr">
+      <c r="F162" s="9" t="inlineStr"/>
+      <c r="G162" s="9" t="inlineStr"/>
+      <c r="H162" s="13" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I162" s="17" t="inlineStr">
+      <c r="I162" s="9" t="inlineStr">
         <is>
           <t>70775</t>
         </is>
       </c>
-      <c r="J162" s="22" t="inlineStr">
+      <c r="J162" s="14" t="inlineStr">
         <is>
           <t>4000000</t>
         </is>
       </c>
-      <c r="K162" s="17" t="inlineStr"/>
-      <c r="L162" s="17" t="inlineStr">
+      <c r="K162" s="9" t="inlineStr"/>
+      <c r="L162" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="17" t="inlineStr">
+      <c r="A163" s="9" t="inlineStr">
         <is>
           <t>M023</t>
         </is>
       </c>
-      <c r="B163" s="18" t="inlineStr">
+      <c r="B163" s="10" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 4000000.00
 Borrower Amount: 4000000.00</t>
         </is>
       </c>
-      <c r="C163" s="17" t="inlineStr"/>
-      <c r="D163" s="17" t="inlineStr"/>
-      <c r="E163" s="23" t="inlineStr">
+      <c r="C163" s="9" t="inlineStr"/>
+      <c r="D163" s="9" t="inlineStr"/>
+      <c r="E163" s="15" t="inlineStr">
         <is>
           <t>Interunit Fund Transfer as Inter Unit Loan A/C-Transformer Unit, MDB#0313</t>
         </is>
       </c>
-      <c r="F163" s="17" t="inlineStr"/>
-      <c r="G163" s="17" t="inlineStr"/>
-      <c r="H163" s="17" t="inlineStr"/>
-      <c r="I163" s="17" t="inlineStr"/>
-      <c r="J163" s="17" t="inlineStr"/>
-      <c r="K163" s="17" t="inlineStr"/>
-      <c r="L163" s="17" t="inlineStr">
+      <c r="F163" s="9" t="inlineStr"/>
+      <c r="G163" s="9" t="inlineStr"/>
+      <c r="H163" s="9" t="inlineStr"/>
+      <c r="I163" s="9" t="inlineStr"/>
+      <c r="J163" s="9" t="inlineStr"/>
+      <c r="K163" s="9" t="inlineStr"/>
+      <c r="L163" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="17" t="inlineStr">
+      <c r="A164" s="9" t="inlineStr">
         <is>
           <t>M023</t>
         </is>
       </c>
-      <c r="B164" s="18" t="inlineStr"/>
-      <c r="C164" s="17" t="inlineStr"/>
-      <c r="D164" s="17" t="inlineStr">
+      <c r="B164" s="10" t="inlineStr"/>
+      <c r="C164" s="9" t="inlineStr"/>
+      <c r="D164" s="9" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E164" s="24" t="inlineStr">
+      <c r="E164" s="16" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F164" s="17" t="inlineStr"/>
-      <c r="G164" s="17" t="inlineStr"/>
-      <c r="H164" s="17" t="inlineStr"/>
-      <c r="I164" s="17" t="inlineStr"/>
-      <c r="J164" s="17" t="inlineStr"/>
-      <c r="K164" s="17" t="inlineStr"/>
-      <c r="L164" s="17" t="inlineStr">
+      <c r="F164" s="9" t="inlineStr"/>
+      <c r="G164" s="9" t="inlineStr"/>
+      <c r="H164" s="9" t="inlineStr"/>
+      <c r="I164" s="9" t="inlineStr"/>
+      <c r="J164" s="9" t="inlineStr"/>
+      <c r="K164" s="9" t="inlineStr"/>
+      <c r="L164" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="9" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
-      <c r="B165" s="10" t="inlineStr"/>
-      <c r="C165" s="11" t="inlineStr">
+      <c r="A165" s="17" t="inlineStr">
+        <is>
+          <t>M056</t>
+        </is>
+      </c>
+      <c r="B165" s="18" t="inlineStr"/>
+      <c r="C165" s="19" t="inlineStr">
         <is>
           <t>26/Jun/2025</t>
         </is>
       </c>
-      <c r="D165" s="9" t="inlineStr">
+      <c r="D165" s="17" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E165" s="12" t="inlineStr">
+      <c r="E165" s="20" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F165" s="9" t="inlineStr"/>
-      <c r="G165" s="9" t="inlineStr"/>
-      <c r="H165" s="13" t="inlineStr">
+      <c r="F165" s="17" t="inlineStr"/>
+      <c r="G165" s="17" t="inlineStr"/>
+      <c r="H165" s="21" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I165" s="9" t="inlineStr">
+      <c r="I165" s="17" t="inlineStr">
         <is>
           <t>70687</t>
         </is>
       </c>
-      <c r="J165" s="14" t="inlineStr">
+      <c r="J165" s="22" t="inlineStr">
         <is>
           <t>5137392</t>
         </is>
       </c>
-      <c r="K165" s="9" t="inlineStr"/>
-      <c r="L165" s="9" t="inlineStr">
+      <c r="K165" s="17" t="inlineStr"/>
+      <c r="L165" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="9" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
-      <c r="B166" s="10" t="inlineStr">
+      <c r="A166" s="17" t="inlineStr">
+        <is>
+          <t>M056</t>
+        </is>
+      </c>
+      <c r="B166" s="18" t="inlineStr">
         <is>
           <t>Manual Match
 Lender Amount: 5137392.00
 Borrower Amount: 5137392.00</t>
         </is>
       </c>
-      <c r="C166" s="9" t="inlineStr"/>
-      <c r="D166" s="9" t="inlineStr"/>
-      <c r="E166" s="15" t="inlineStr">
+      <c r="C166" s="17" t="inlineStr"/>
+      <c r="D166" s="17" t="inlineStr"/>
+      <c r="E166" s="23" t="inlineStr">
         <is>
           <t>Amount paid as interunit vendor payment.(RR Imperial Electricals Limited)</t>
         </is>
       </c>
-      <c r="F166" s="9" t="inlineStr"/>
-      <c r="G166" s="9" t="inlineStr"/>
-      <c r="H166" s="9" t="inlineStr"/>
-      <c r="I166" s="9" t="inlineStr"/>
-      <c r="J166" s="9" t="inlineStr"/>
-      <c r="K166" s="9" t="inlineStr"/>
-      <c r="L166" s="9" t="inlineStr">
+      <c r="F166" s="17" t="inlineStr"/>
+      <c r="G166" s="17" t="inlineStr"/>
+      <c r="H166" s="17" t="inlineStr"/>
+      <c r="I166" s="17" t="inlineStr"/>
+      <c r="J166" s="17" t="inlineStr"/>
+      <c r="K166" s="17" t="inlineStr"/>
+      <c r="L166" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="9" t="inlineStr">
-        <is>
-          <t>M067</t>
-        </is>
-      </c>
-      <c r="B167" s="10" t="inlineStr"/>
-      <c r="C167" s="9" t="inlineStr"/>
-      <c r="D167" s="9" t="inlineStr">
+      <c r="A167" s="17" t="inlineStr">
+        <is>
+          <t>M056</t>
+        </is>
+      </c>
+      <c r="B167" s="18" t="inlineStr"/>
+      <c r="C167" s="17" t="inlineStr"/>
+      <c r="D167" s="17" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E167" s="16" t="inlineStr">
+      <c r="E167" s="24" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F167" s="9" t="inlineStr"/>
-      <c r="G167" s="9" t="inlineStr"/>
-      <c r="H167" s="9" t="inlineStr"/>
-      <c r="I167" s="9" t="inlineStr"/>
-      <c r="J167" s="9" t="inlineStr"/>
-      <c r="K167" s="9" t="inlineStr"/>
-      <c r="L167" s="9" t="inlineStr">
+      <c r="F167" s="17" t="inlineStr"/>
+      <c r="G167" s="17" t="inlineStr"/>
+      <c r="H167" s="17" t="inlineStr"/>
+      <c r="I167" s="17" t="inlineStr"/>
+      <c r="J167" s="17" t="inlineStr"/>
+      <c r="K167" s="17" t="inlineStr"/>
+      <c r="L167" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="17" t="inlineStr">
+      <c r="A168" s="9" t="inlineStr">
         <is>
           <t>M024</t>
         </is>
       </c>
-      <c r="B168" s="18" t="inlineStr"/>
-      <c r="C168" s="19" t="inlineStr">
+      <c r="B168" s="10" t="inlineStr"/>
+      <c r="C168" s="11" t="inlineStr">
         <is>
           <t>29/Jun/2025</t>
         </is>
       </c>
-      <c r="D168" s="17" t="inlineStr">
+      <c r="D168" s="9" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E168" s="20" t="inlineStr">
+      <c r="E168" s="12" t="inlineStr">
         <is>
           <t>(as per details)</t>
         </is>
       </c>
-      <c r="F168" s="17" t="inlineStr"/>
-      <c r="G168" s="17" t="inlineStr"/>
-      <c r="H168" s="21" t="inlineStr">
+      <c r="F168" s="9" t="inlineStr"/>
+      <c r="G168" s="9" t="inlineStr"/>
+      <c r="H168" s="13" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I168" s="17" t="inlineStr">
+      <c r="I168" s="9" t="inlineStr">
         <is>
           <t>70593</t>
         </is>
       </c>
-      <c r="J168" s="22" t="inlineStr">
+      <c r="J168" s="14" t="inlineStr">
         <is>
           <t>400000</t>
         </is>
       </c>
-      <c r="K168" s="17" t="inlineStr"/>
-      <c r="L168" s="17" t="inlineStr">
+      <c r="K168" s="9" t="inlineStr"/>
+      <c r="L168" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="17" t="inlineStr">
+      <c r="A169" s="9" t="inlineStr">
         <is>
           <t>M024</t>
         </is>
       </c>
-      <c r="B169" s="18" t="inlineStr"/>
-      <c r="C169" s="17" t="inlineStr"/>
-      <c r="D169" s="17" t="inlineStr"/>
-      <c r="E169" s="20" t="inlineStr">
+      <c r="B169" s="10" t="inlineStr"/>
+      <c r="C169" s="9" t="inlineStr"/>
+      <c r="D169" s="9" t="inlineStr"/>
+      <c r="E169" s="12" t="inlineStr">
         <is>
           <t>Inter Unit Loan A/C-Dredging Unit</t>
         </is>
       </c>
-      <c r="F169" s="17" t="inlineStr"/>
-      <c r="G169" s="17" t="inlineStr"/>
-      <c r="H169" s="17" t="inlineStr"/>
-      <c r="I169" s="17" t="inlineStr"/>
-      <c r="J169" s="22" t="inlineStr">
+      <c r="F169" s="9" t="inlineStr"/>
+      <c r="G169" s="9" t="inlineStr"/>
+      <c r="H169" s="9" t="inlineStr"/>
+      <c r="I169" s="9" t="inlineStr"/>
+      <c r="J169" s="14" t="inlineStr">
         <is>
           <t>3000000</t>
         </is>
       </c>
-      <c r="K169" s="17" t="inlineStr"/>
-      <c r="L169" s="17" t="inlineStr">
+      <c r="K169" s="9" t="inlineStr"/>
+      <c r="L169" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="17" t="inlineStr">
+      <c r="A170" s="9" t="inlineStr">
         <is>
           <t>M024</t>
         </is>
       </c>
-      <c r="B170" s="18" t="inlineStr"/>
-      <c r="C170" s="17" t="inlineStr"/>
-      <c r="D170" s="17" t="inlineStr"/>
-      <c r="E170" s="20" t="inlineStr">
+      <c r="B170" s="10" t="inlineStr"/>
+      <c r="C170" s="9" t="inlineStr"/>
+      <c r="D170" s="9" t="inlineStr"/>
+      <c r="E170" s="12" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F170" s="17" t="inlineStr"/>
-      <c r="G170" s="17" t="inlineStr"/>
-      <c r="H170" s="17" t="inlineStr"/>
-      <c r="I170" s="17" t="inlineStr"/>
-      <c r="J170" s="17" t="inlineStr"/>
-      <c r="K170" s="22" t="inlineStr">
+      <c r="F170" s="9" t="inlineStr"/>
+      <c r="G170" s="9" t="inlineStr"/>
+      <c r="H170" s="9" t="inlineStr"/>
+      <c r="I170" s="9" t="inlineStr"/>
+      <c r="J170" s="9" t="inlineStr"/>
+      <c r="K170" s="14" t="inlineStr">
         <is>
           <t>400000</t>
         </is>
       </c>
-      <c r="L170" s="17" t="inlineStr">
+      <c r="L170" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="17" t="inlineStr">
+      <c r="A171" s="9" t="inlineStr">
         <is>
           <t>M024</t>
         </is>
       </c>
-      <c r="B171" s="18" t="inlineStr"/>
-      <c r="C171" s="17" t="inlineStr"/>
-      <c r="D171" s="17" t="inlineStr"/>
-      <c r="E171" s="20" t="inlineStr">
+      <c r="B171" s="10" t="inlineStr"/>
+      <c r="C171" s="9" t="inlineStr"/>
+      <c r="D171" s="9" t="inlineStr"/>
+      <c r="E171" s="12" t="inlineStr">
         <is>
           <t>Midland-CE-0011-1060000331-CI</t>
         </is>
       </c>
-      <c r="F171" s="17" t="inlineStr"/>
-      <c r="G171" s="17" t="inlineStr"/>
-      <c r="H171" s="17" t="inlineStr"/>
-      <c r="I171" s="17" t="inlineStr"/>
-      <c r="J171" s="17" t="inlineStr"/>
-      <c r="K171" s="22" t="inlineStr">
+      <c r="F171" s="9" t="inlineStr"/>
+      <c r="G171" s="9" t="inlineStr"/>
+      <c r="H171" s="9" t="inlineStr"/>
+      <c r="I171" s="9" t="inlineStr"/>
+      <c r="J171" s="9" t="inlineStr"/>
+      <c r="K171" s="14" t="inlineStr">
         <is>
           <t>3000000</t>
         </is>
       </c>
-      <c r="L171" s="17" t="inlineStr">
+      <c r="L171" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="17" t="inlineStr">
+      <c r="A172" s="9" t="inlineStr">
         <is>
           <t>M024</t>
         </is>
       </c>
-      <c r="B172" s="18" t="inlineStr">
+      <c r="B172" s="10" t="inlineStr">
         <is>
           <t>Interunit Loan Match: MDB#0331
 Lender Amount: 400000.00
 Borrower Amount: 400000.00</t>
         </is>
       </c>
-      <c r="C172" s="17" t="inlineStr"/>
-      <c r="D172" s="17" t="inlineStr"/>
-      <c r="E172" s="23" t="inlineStr">
+      <c r="C172" s="9" t="inlineStr"/>
+      <c r="D172" s="9" t="inlineStr"/>
+      <c r="E172" s="15" t="inlineStr">
         <is>
           <t>Interunit fund Transfer as Inter Unit Loan A/C-Transformer Unit, MDB#0313 &amp; Inter Unit Loan A/C-Dredging Unit, MDB#0322</t>
         </is>
       </c>
-      <c r="F172" s="17" t="inlineStr"/>
-      <c r="G172" s="17" t="inlineStr"/>
-      <c r="H172" s="17" t="inlineStr"/>
-      <c r="I172" s="17" t="inlineStr"/>
-      <c r="J172" s="17" t="inlineStr"/>
-      <c r="K172" s="17" t="inlineStr"/>
-      <c r="L172" s="17" t="inlineStr">
+      <c r="F172" s="9" t="inlineStr"/>
+      <c r="G172" s="9" t="inlineStr"/>
+      <c r="H172" s="9" t="inlineStr"/>
+      <c r="I172" s="9" t="inlineStr"/>
+      <c r="J172" s="9" t="inlineStr"/>
+      <c r="K172" s="9" t="inlineStr"/>
+      <c r="L172" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="17" t="inlineStr">
+      <c r="A173" s="9" t="inlineStr">
         <is>
           <t>M024</t>
         </is>
       </c>
-      <c r="B173" s="18" t="inlineStr"/>
-      <c r="C173" s="17" t="inlineStr"/>
-      <c r="D173" s="17" t="inlineStr">
+      <c r="B173" s="10" t="inlineStr"/>
+      <c r="C173" s="9" t="inlineStr"/>
+      <c r="D173" s="9" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E173" s="24" t="inlineStr">
+      <c r="E173" s="16" t="inlineStr">
         <is>
           <t>ashiq</t>
         </is>
       </c>
-      <c r="F173" s="17" t="inlineStr"/>
-      <c r="G173" s="17" t="inlineStr"/>
-      <c r="H173" s="17" t="inlineStr"/>
-      <c r="I173" s="17" t="inlineStr"/>
-      <c r="J173" s="17" t="inlineStr"/>
-      <c r="K173" s="17" t="inlineStr"/>
-      <c r="L173" s="17" t="inlineStr">
+      <c r="F173" s="9" t="inlineStr"/>
+      <c r="G173" s="9" t="inlineStr"/>
+      <c r="H173" s="9" t="inlineStr"/>
+      <c r="I173" s="9" t="inlineStr"/>
+      <c r="J173" s="9" t="inlineStr"/>
+      <c r="K173" s="9" t="inlineStr"/>
+      <c r="L173" s="9" t="inlineStr">
         <is>
           <t>Interunit</t>
         </is>
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="9" t="inlineStr">
-        <is>
-          <t>M068</t>
-        </is>
-      </c>
-      <c r="B174" s="10" t="inlineStr"/>
-      <c r="C174" s="11" t="inlineStr">
+      <c r="A174" s="17" t="inlineStr">
+        <is>
+          <t>M057</t>
+        </is>
+      </c>
+      <c r="B174" s="18" t="inlineStr"/>
+      <c r="C174" s="19" t="inlineStr">
         <is>
           <t>29/Jun/2025</t>
         </is>
       </c>
-      <c r="D174" s="9" t="inlineStr">
+      <c r="D174" s="17" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="E174" s="12" t="inlineStr">
+      <c r="E174" s="20" t="inlineStr">
         <is>
           <t>Mutual Trust Bank Ltd-SND-002-0320004355</t>
         </is>
       </c>
-      <c r="F174" s="9" t="inlineStr"/>
-      <c r="G174" s="9" t="inlineStr"/>
-      <c r="H174" s="13" t="inlineStr">
+      <c r="F174" s="17" t="inlineStr"/>
+      <c r="G174" s="17" t="inlineStr"/>
+      <c r="H174" s="21" t="inlineStr">
         <is>
           <t>Bank Payment</t>
         </is>
       </c>
-      <c r="I174" s="9" t="inlineStr">
+      <c r="I174" s="17" t="inlineStr">
         <is>
           <t>70686</t>
         </is>
       </c>
-      <c r="J174" s="14" t="inlineStr">
+      <c r="J174" s="22" t="inlineStr">
         <is>
           <t>11780452</t>
         </is>
       </c>
-      <c r="K174" s="9" t="inlineStr"/>
-      <c r="L174" s="9" t="inlineStr">
+      <c r="K174" s="17" t="inlineStr"/>
+      <c r="L174" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="9" t="inlineStr">
-        <is>
-          <t>M068</t>
-        </is>
-      </c>
-      <c r="B175" s="10" t="inlineStr">
+      <c r="A175" s="17" t="inlineStr">
+        <is>
+          <t>M057</t>
+        </is>
+      </c>
+      <c r="B175" s="18" t="inlineStr">
         <is>
           <t>Manual Match
 Lender Amount: 11780452.00
 Borrower Amount: 11780452.00</t>
         </is>
       </c>
-      <c r="C175" s="9" t="inlineStr"/>
-      <c r="D175" s="9" t="inlineStr"/>
-      <c r="E175" s="15" t="inlineStr">
+      <c r="C175" s="17" t="inlineStr"/>
+      <c r="D175" s="17" t="inlineStr"/>
+      <c r="E175" s="23" t="inlineStr">
         <is>
           <t>Amount paid as Inter Unit Loan A/C-Transformer Unit (Rangpur Metal Industries Ltd.)</t>
         </is>
       </c>
-      <c r="F175" s="9" t="inlineStr"/>
-      <c r="G175" s="9" t="inlineStr"/>
-      <c r="H175" s="9" t="inlineStr"/>
-      <c r="I175" s="9" t="inlineStr"/>
-      <c r="J175" s="9" t="inlineStr"/>
-      <c r="K175" s="9" t="inlineStr"/>
-      <c r="L175" s="9" t="inlineStr">
+      <c r="F175" s="17" t="inlineStr"/>
+      <c r="G175" s="17" t="inlineStr"/>
+      <c r="H175" s="17" t="inlineStr"/>
+      <c r="I175" s="17" t="inlineStr"/>
+      <c r="J175" s="17" t="inlineStr"/>
+      <c r="K175" s="17" t="inlineStr"/>
+      <c r="L175" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="9" t="inlineStr">
-        <is>
-          <t>M068</t>
-        </is>
-      </c>
-      <c r="B176" s="10" t="inlineStr"/>
-      <c r="C176" s="9" t="inlineStr"/>
-      <c r="D176" s="9" t="inlineStr">
+      <c r="A176" s="17" t="inlineStr">
+        <is>
+          <t>M057</t>
+        </is>
+      </c>
+      <c r="B176" s="18" t="inlineStr"/>
+      <c r="C176" s="17" t="inlineStr"/>
+      <c r="D176" s="17" t="inlineStr">
         <is>
           <t>Entered By :</t>
         </is>
       </c>
-      <c r="E176" s="16" t="inlineStr">
+      <c r="E176" s="24" t="inlineStr">
         <is>
           <t>sayeda</t>
         </is>
       </c>
-      <c r="F176" s="9" t="inlineStr"/>
-      <c r="G176" s="9" t="inlineStr"/>
-      <c r="H176" s="9" t="inlineStr"/>
-      <c r="I176" s="9" t="inlineStr"/>
-      <c r="J176" s="9" t="inlineStr"/>
-      <c r="K176" s="9" t="inlineStr"/>
-      <c r="L176" s="9" t="inlineStr">
+      <c r="F176" s="17" t="inlineStr"/>
+      <c r="G176" s="17" t="inlineStr"/>
+      <c r="H176" s="17" t="inlineStr"/>
+      <c r="I176" s="17" t="inlineStr"/>
+      <c r="J176" s="17" t="inlineStr"/>
+      <c r="K176" s="17" t="inlineStr"/>
+      <c r="L176" s="17" t="inlineStr">
         <is>
           <t>Manual</t>
         </is>
@@ -6711,7 +6544,7 @@
       <c r="H177" s="1" t="inlineStr"/>
       <c r="I177" s="1" t="inlineStr"/>
       <c r="J177" s="1" t="inlineStr"/>
-      <c r="K177" s="25" t="inlineStr">
+      <c r="K177" s="28" t="inlineStr">
         <is>
           <t>95590149.25</t>
         </is>
@@ -6759,7 +6592,7 @@
       <c r="H179" s="1" t="inlineStr"/>
       <c r="I179" s="1" t="inlineStr"/>
       <c r="J179" s="1" t="inlineStr"/>
-      <c r="K179" s="25" t="inlineStr">
+      <c r="K179" s="28" t="inlineStr">
         <is>
           <t>95590149.25</t>
         </is>

</xml_diff>